<commit_message>
feat: reading Pilot Cards (first Half) from excel now working.
</commit_message>
<xml_diff>
--- a/VadersLittleHelper/db/ComponentDB.xlsx
+++ b/VadersLittleHelper/db/ComponentDB.xlsx
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="37">
   <si>
     <t>Ship</t>
   </si>
@@ -112,9 +112,6 @@
     <t>Unique</t>
   </si>
   <si>
-    <t>Limited</t>
-  </si>
-  <si>
     <t>He does Stuff</t>
   </si>
   <si>
@@ -137,6 +134,9 @@
   </si>
   <si>
     <t>Imperial</t>
+  </si>
+  <si>
+    <t>He's Just a Guy</t>
   </si>
 </sst>
 </file>
@@ -604,10 +604,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{258C231B-D951-459D-84CF-A781BDBA3B3B}">
-  <dimension ref="A1:G4"/>
+  <dimension ref="A1:F4"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="H4" sqref="H4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -616,7 +616,7 @@
     <col min="3" max="3" width="14.5546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>2</v>
       </c>
@@ -627,24 +627,21 @@
         <v>3</v>
       </c>
       <c r="D1" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="E1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="F1" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>16</v>
       </c>
       <c r="B2" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C2">
         <v>30</v>
@@ -653,56 +650,50 @@
         <v>30</v>
       </c>
       <c r="E2" t="s">
+        <v>29</v>
+      </c>
+      <c r="F2" t="s">
         <v>17</v>
       </c>
-      <c r="F2" t="s">
-        <v>31</v>
-      </c>
-      <c r="G2" t="s">
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
+      <c r="B3" t="s">
         <v>33</v>
-      </c>
-      <c r="B3" t="s">
-        <v>34</v>
       </c>
       <c r="C3">
         <v>33</v>
       </c>
       <c r="D3" t="s">
+        <v>30</v>
+      </c>
+      <c r="E3" t="s">
         <v>13</v>
       </c>
-      <c r="E3" t="s">
+      <c r="F3" t="s">
         <v>18</v>
       </c>
-      <c r="F3" t="s">
-        <v>31</v>
-      </c>
-      <c r="G3" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>35</v>
+        <v>34</v>
+      </c>
+      <c r="B4" t="s">
+        <v>36</v>
       </c>
       <c r="C4">
         <v>15</v>
       </c>
       <c r="D4" t="s">
+        <v>31</v>
+      </c>
+      <c r="E4" t="s">
         <v>7</v>
       </c>
-      <c r="E4" t="s">
-        <v>36</v>
-      </c>
       <c r="F4" t="s">
-        <v>32</v>
-      </c>
-      <c r="G4" t="s">
-        <v>32</v>
+        <v>35</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Upgrade datahandling for Pilots, implement basic handling for Upgrades and Ships
</commit_message>
<xml_diff>
--- a/VadersLittleHelper/db/ComponentDB.xlsx
+++ b/VadersLittleHelper/db/ComponentDB.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="5292" windowHeight="5796" activeTab="1" xr2:uid="{EFCB0871-0F77-484A-948E-5B1FEFF48867}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="5292" windowHeight="5796" activeTab="2" xr2:uid="{EFCB0871-0F77-484A-948E-5B1FEFF48867}"/>
   </bookViews>
   <sheets>
     <sheet name="ShipDB" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="65">
   <si>
     <t>Ship</t>
   </si>
@@ -137,6 +137,90 @@
   </si>
   <si>
     <t>He's Just a Guy</t>
+  </si>
+  <si>
+    <t>Id</t>
+  </si>
+  <si>
+    <t>PilotSkill</t>
+  </si>
+  <si>
+    <t>Firepower</t>
+  </si>
+  <si>
+    <t>Agility</t>
+  </si>
+  <si>
+    <t>Hull</t>
+  </si>
+  <si>
+    <t>Shields</t>
+  </si>
+  <si>
+    <t>P0001</t>
+  </si>
+  <si>
+    <t>P0002</t>
+  </si>
+  <si>
+    <t>P0003</t>
+  </si>
+  <si>
+    <t>U0001</t>
+  </si>
+  <si>
+    <t>U0002</t>
+  </si>
+  <si>
+    <t>U0003</t>
+  </si>
+  <si>
+    <t>U0004</t>
+  </si>
+  <si>
+    <t>Limited</t>
+  </si>
+  <si>
+    <t>Woooo</t>
+  </si>
+  <si>
+    <t>Pew pew</t>
+  </si>
+  <si>
+    <t>Go Wroom</t>
+  </si>
+  <si>
+    <t>Spacecoke</t>
+  </si>
+  <si>
+    <t>S0001</t>
+  </si>
+  <si>
+    <t>S0002</t>
+  </si>
+  <si>
+    <t>S0003</t>
+  </si>
+  <si>
+    <t>S0004</t>
+  </si>
+  <si>
+    <t>S0005</t>
+  </si>
+  <si>
+    <t>S0006</t>
+  </si>
+  <si>
+    <t>S0007</t>
+  </si>
+  <si>
+    <t>S0008</t>
+  </si>
+  <si>
+    <t>S0009</t>
+  </si>
+  <si>
+    <t>S0010</t>
   </si>
 </sst>
 </file>
@@ -497,102 +581,135 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3F9499D8-5CE4-4AC7-B597-31CD0CBB4E0C}">
-  <dimension ref="A1:B11"/>
+  <dimension ref="A1:C11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A12" sqref="A12"/>
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="36.88671875" customWidth="1"/>
+    <col min="2" max="2" width="36.88671875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C1" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
+        <v>55</v>
+      </c>
+      <c r="B2" t="s">
         <v>6</v>
       </c>
-      <c r="B2">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
+        <v>56</v>
+      </c>
+      <c r="B3" t="s">
         <v>7</v>
       </c>
-      <c r="B3">
+      <c r="C3">
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
+        <v>57</v>
+      </c>
+      <c r="B4" t="s">
         <v>8</v>
       </c>
-      <c r="B4">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C4">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
+        <v>58</v>
+      </c>
+      <c r="B5" t="s">
         <v>9</v>
       </c>
-      <c r="B5">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C5">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
+        <v>59</v>
+      </c>
+      <c r="B6" t="s">
         <v>10</v>
       </c>
-      <c r="B6">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
+        <v>60</v>
+      </c>
+      <c r="B7" t="s">
         <v>11</v>
       </c>
-      <c r="B7">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C7">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
+        <v>61</v>
+      </c>
+      <c r="B8" t="s">
         <v>12</v>
       </c>
-      <c r="B8">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C8">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
+        <v>62</v>
+      </c>
+      <c r="B9" t="s">
         <v>13</v>
       </c>
-      <c r="B9">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
+        <v>63</v>
+      </c>
+      <c r="B10" t="s">
         <v>14</v>
       </c>
-      <c r="B10">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
+        <v>64</v>
+      </c>
+      <c r="B11" t="s">
         <v>15</v>
       </c>
-      <c r="B11">
+      <c r="C11">
         <v>1</v>
       </c>
     </row>
@@ -604,96 +721,180 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{258C231B-D951-459D-84CF-A781BDBA3B3B}">
-  <dimension ref="A1:F4"/>
+  <dimension ref="A1:M4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+    <sheetView topLeftCell="I1" workbookViewId="0">
+      <selection activeCell="M5" sqref="M5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="2" width="26.6640625" customWidth="1"/>
-    <col min="3" max="3" width="14.5546875" customWidth="1"/>
+    <col min="2" max="3" width="26.6640625" customWidth="1"/>
+    <col min="4" max="4" width="14.5546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
-        <v>2</v>
+        <v>37</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="H1" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
+        <v>43</v>
+      </c>
+      <c r="B2" t="s">
         <v>16</v>
       </c>
-      <c r="B2" t="s">
+      <c r="C2" t="s">
         <v>28</v>
       </c>
-      <c r="C2">
+      <c r="D2">
         <v>30</v>
       </c>
-      <c r="D2" t="s">
+      <c r="E2" t="s">
         <v>30</v>
       </c>
-      <c r="E2" t="s">
+      <c r="F2" t="s">
         <v>29</v>
       </c>
-      <c r="F2" t="s">
+      <c r="G2" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="H2">
+        <v>8</v>
+      </c>
+      <c r="I2">
+        <v>3</v>
+      </c>
+      <c r="J2">
+        <v>2</v>
+      </c>
+      <c r="K2">
+        <v>2</v>
+      </c>
+      <c r="L2">
+        <v>2</v>
+      </c>
+      <c r="M2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
+        <v>44</v>
+      </c>
+      <c r="B3" t="s">
         <v>32</v>
       </c>
-      <c r="B3" t="s">
+      <c r="C3" t="s">
         <v>33</v>
       </c>
-      <c r="C3">
+      <c r="D3">
         <v>33</v>
       </c>
-      <c r="D3" t="s">
+      <c r="E3" t="s">
         <v>30</v>
       </c>
-      <c r="E3" t="s">
+      <c r="F3" t="s">
         <v>13</v>
       </c>
-      <c r="F3" t="s">
+      <c r="G3" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="H3">
+        <v>7</v>
+      </c>
+      <c r="I3">
+        <v>3</v>
+      </c>
+      <c r="J3">
+        <v>1</v>
+      </c>
+      <c r="K3">
+        <v>5</v>
+      </c>
+      <c r="L3">
+        <v>5</v>
+      </c>
+      <c r="M3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
+        <v>45</v>
+      </c>
+      <c r="B4" t="s">
         <v>34</v>
       </c>
-      <c r="B4" t="s">
+      <c r="C4" t="s">
         <v>36</v>
       </c>
-      <c r="C4">
+      <c r="D4">
         <v>15</v>
       </c>
-      <c r="D4" t="s">
+      <c r="E4" t="s">
         <v>31</v>
       </c>
-      <c r="E4" t="s">
+      <c r="F4" t="s">
         <v>7</v>
       </c>
-      <c r="F4" t="s">
+      <c r="G4" t="s">
         <v>35</v>
+      </c>
+      <c r="H4">
+        <v>2</v>
+      </c>
+      <c r="I4">
+        <v>2</v>
+      </c>
+      <c r="J4">
+        <v>3</v>
+      </c>
+      <c r="K4">
+        <v>2</v>
+      </c>
+      <c r="L4">
+        <v>1</v>
+      </c>
+      <c r="M4">
+        <v>2</v>
       </c>
     </row>
   </sheetData>
@@ -704,81 +905,141 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{18EF0634-2CFE-451C-B280-271F73D0B3E3}">
-  <dimension ref="A1:D5"/>
+  <dimension ref="A1:H5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H6" sqref="H6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
-        <v>2</v>
+        <v>37</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="G1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="C1" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="H1" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
+        <v>46</v>
+      </c>
+      <c r="B2" t="s">
         <v>19</v>
       </c>
-      <c r="B2" t="s">
+      <c r="C2" t="s">
+        <v>51</v>
+      </c>
+      <c r="D2">
+        <v>1</v>
+      </c>
+      <c r="E2" t="s">
+        <v>31</v>
+      </c>
+      <c r="F2" t="s">
+        <v>31</v>
+      </c>
+      <c r="G2" t="s">
         <v>20</v>
       </c>
-      <c r="C2">
-        <v>1</v>
-      </c>
-      <c r="D2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="H2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
+        <v>47</v>
+      </c>
+      <c r="B3" t="s">
         <v>21</v>
       </c>
-      <c r="B3" t="s">
+      <c r="C3" t="s">
+        <v>52</v>
+      </c>
+      <c r="D3">
+        <v>1</v>
+      </c>
+      <c r="E3" t="s">
+        <v>31</v>
+      </c>
+      <c r="F3" t="s">
+        <v>31</v>
+      </c>
+      <c r="G3" t="s">
         <v>20</v>
       </c>
-      <c r="C3">
-        <v>1</v>
-      </c>
-      <c r="D3">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="H3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
+        <v>48</v>
+      </c>
+      <c r="B4" t="s">
         <v>22</v>
       </c>
-      <c r="B4" t="s">
+      <c r="C4" t="s">
+        <v>53</v>
+      </c>
+      <c r="D4">
+        <v>2</v>
+      </c>
+      <c r="E4" t="s">
+        <v>31</v>
+      </c>
+      <c r="F4" t="s">
+        <v>30</v>
+      </c>
+      <c r="G4" t="s">
         <v>23</v>
       </c>
-      <c r="C4">
-        <v>2</v>
-      </c>
-      <c r="D4">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="H4">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
+        <v>49</v>
+      </c>
+      <c r="B5" t="s">
         <v>24</v>
       </c>
-      <c r="B5" t="s">
+      <c r="C5" t="s">
+        <v>54</v>
+      </c>
+      <c r="D5">
+        <v>2</v>
+      </c>
+      <c r="E5" t="s">
+        <v>31</v>
+      </c>
+      <c r="F5" t="s">
+        <v>31</v>
+      </c>
+      <c r="G5" t="s">
         <v>25</v>
       </c>
-      <c r="C5">
-        <v>2</v>
-      </c>
-      <c r="D5">
+      <c r="H5">
         <v>1</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Populated excel db with Update Cards.
</commit_message>
<xml_diff>
--- a/VadersLittleHelper/db/ComponentDB.xlsx
+++ b/VadersLittleHelper/db/ComponentDB.xlsx
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="65">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="482" uniqueCount="272">
   <si>
     <t>Ship</t>
   </si>
@@ -91,9 +91,6 @@
     <t>Elite Pilot Skill</t>
   </si>
   <si>
-    <t>Crackshot</t>
-  </si>
-  <si>
     <t>Vectored Thrusters</t>
   </si>
   <si>
@@ -181,18 +178,6 @@
     <t>Limited</t>
   </si>
   <si>
-    <t>Woooo</t>
-  </si>
-  <si>
-    <t>Pew pew</t>
-  </si>
-  <si>
-    <t>Go Wroom</t>
-  </si>
-  <si>
-    <t>Spacecoke</t>
-  </si>
-  <si>
     <t>S0001</t>
   </si>
   <si>
@@ -221,6 +206,642 @@
   </si>
   <si>
     <t>S0010</t>
+  </si>
+  <si>
+    <t>A-Wing Test Pilot</t>
+  </si>
+  <si>
+    <t>Title</t>
+  </si>
+  <si>
+    <t>Alliance Overhaul</t>
+  </si>
+  <si>
+    <t>A-WING ONLY. Your upgrade bar gains one ELITE icon. You cannot equip 2 of the same ELITE upgrade cards. You cannot Equip this card if your pilot skill value is '1' or lower.</t>
+  </si>
+  <si>
+    <t>ARC-170 ONLY. When attacking with a primary weapon from your primary firing arc, you may roll 1 additional attack die. When attacking from your auxiliary arc, you may change one of your FOCUS result to a CRITICAL result.</t>
+  </si>
+  <si>
+    <t>Adaptive Ailerons</t>
+  </si>
+  <si>
+    <t>TIE STRIKER ONLY. Immediately before you reveal your dial, if you are not stressed, you MUST execute a white [bank left 1], [forward 1] or [bank right 1] maneuver.</t>
+  </si>
+  <si>
+    <t>TIE/x7</t>
+  </si>
+  <si>
+    <t>TIE/D</t>
+  </si>
+  <si>
+    <t>TIE DEFENDER ONLY. Once per round, after you attack with a CANNON secondary weapon taht costs 3 or fewer squad points, you may perform a primary weapon attack.</t>
+  </si>
+  <si>
+    <t>TIE Shuttle</t>
+  </si>
+  <si>
+    <t>BTL-A4 Y-Wing</t>
+  </si>
+  <si>
+    <t>Y-WING ONLY. You cannot attack ships outside your firing arc. After you perform a primary attack, you may immediately perform an attack with a TURRET secondary weapon.</t>
+  </si>
+  <si>
+    <t>Andrasta</t>
+  </si>
+  <si>
+    <t>FIRESPRAY-31 ONLY. Your upgrade bar gains two additional BOMB icons.</t>
+  </si>
+  <si>
+    <t>Hound's Tooth</t>
+  </si>
+  <si>
+    <t>YV-666 ONLY. After you are destroyed, before you are removed from the play area, you may DEPLOY the Nashtah Pup pilot. It cannot attack this round.</t>
+  </si>
+  <si>
+    <t>Mist Hunter</t>
+  </si>
+  <si>
+    <t>G-1A STARFIGHTER ONLY. Your action bar gains the BARREL ROLL icon. You MUST equip 1 'Tractor Beam' upgrade card (paying ist squad point cost as normal).</t>
+  </si>
+  <si>
+    <t>Concord Dawn Protector</t>
+  </si>
+  <si>
+    <t>PROTECTORATE STARFIGHTER ONLY. When defending, if you are inside the attackers firing arc and at Range 1 and the attacker is inside your firing arc, add 1 EVADE result.</t>
+  </si>
+  <si>
+    <t>TIE BOMBER ONLY. Your upgrade bar loses all TORPEDO, MISSILE and BOMB upgrade icons, and gains 2 CREW upgrade icons. You cannot equip a CREW upgrade card that costs more than 4 squad points.</t>
+  </si>
+  <si>
+    <t>TIE DEFENDER ONLY. Your upgrade bar loses the CANNON and MISSILE upgrade icons. After executing a 3-, 4-, or 5-speed maneuver, you may assign 1 evade token to your ship.</t>
+  </si>
+  <si>
+    <t>System</t>
+  </si>
+  <si>
+    <t>U0005</t>
+  </si>
+  <si>
+    <t>U0006</t>
+  </si>
+  <si>
+    <t>U0007</t>
+  </si>
+  <si>
+    <t>U0008</t>
+  </si>
+  <si>
+    <t>U0009</t>
+  </si>
+  <si>
+    <t>U0010</t>
+  </si>
+  <si>
+    <t>U0011</t>
+  </si>
+  <si>
+    <t>Fire-Control System</t>
+  </si>
+  <si>
+    <t>After you perform an attack, you may acquire a target lock on the defender.</t>
+  </si>
+  <si>
+    <t>Enhanced Scopes</t>
+  </si>
+  <si>
+    <t>During the Activation phase, treat your pilot skill value as '0'.</t>
+  </si>
+  <si>
+    <t>Electronic Baffle</t>
+  </si>
+  <si>
+    <t>When you receive a stress token or an ion token, you may suffer 1 damage to discard that token.</t>
+  </si>
+  <si>
+    <t>Weapons Guidance</t>
+  </si>
+  <si>
+    <t>When attacking, you may spend 1 FOCUS token to change 1 of your blank results to a HIT result.</t>
+  </si>
+  <si>
+    <t>Tech</t>
+  </si>
+  <si>
+    <t>Comm Relay</t>
+  </si>
+  <si>
+    <t>You cannot ever have more than 1 evade token. During the End phase, do not remove an unused evade token from your ship.</t>
+  </si>
+  <si>
+    <t>BB-8</t>
+  </si>
+  <si>
+    <t>When you reveal a green maneuver, you may perform a free barrel roll action.</t>
+  </si>
+  <si>
+    <t>Astromech</t>
+  </si>
+  <si>
+    <t>Targeting Astromech</t>
+  </si>
+  <si>
+    <t>After you execute a red maneuver, you may aquire a target lock.</t>
+  </si>
+  <si>
+    <t>R5-X3</t>
+  </si>
+  <si>
+    <t>Before you reveal your maneuver, you may discard this card to ignore obstacles until the end of the round.</t>
+  </si>
+  <si>
+    <t>R3 Astromech</t>
+  </si>
+  <si>
+    <t>Once per round, when attacking with a primary weapon, you may cancel 1 of your FOCUS results during the 'Modify Attack Dice' step to assign 1 evade token to your ship.</t>
+  </si>
+  <si>
+    <t>R4 Agromech</t>
+  </si>
+  <si>
+    <t>When attacking, after you spend a focus token, you may aquire a target lock on the defender.</t>
+  </si>
+  <si>
+    <t>Salvaged Astromech</t>
+  </si>
+  <si>
+    <t>R4-B11</t>
+  </si>
+  <si>
+    <t>When attacking, if you have a target lock on the defender, you may spend the target lock to choose any or all defense dice. The defender must reroll the chosen dice.</t>
+  </si>
+  <si>
+    <t>"Genius"</t>
+  </si>
+  <si>
+    <t>If you are equipped with a bomb that can be dropped when you reveal your maneuver, you may drop the bomb AFTER you execute your maneuver instead.</t>
+  </si>
+  <si>
+    <t>When you are dealt a Damage card with the SHIP trait, you may immediately discard that card (before resolving its effect). Then, discard this Upgrade card.</t>
+  </si>
+  <si>
+    <t>Unhinged Astromech</t>
+  </si>
+  <si>
+    <t>You may treat all 3-speed maneuvers as green maneuvers.</t>
+  </si>
+  <si>
+    <t>U0012</t>
+  </si>
+  <si>
+    <t>U0013</t>
+  </si>
+  <si>
+    <t>U0014</t>
+  </si>
+  <si>
+    <t>U0015</t>
+  </si>
+  <si>
+    <t>U0016</t>
+  </si>
+  <si>
+    <t>U0017</t>
+  </si>
+  <si>
+    <t>U0018</t>
+  </si>
+  <si>
+    <t>U0019</t>
+  </si>
+  <si>
+    <t>U0020</t>
+  </si>
+  <si>
+    <t>U0021</t>
+  </si>
+  <si>
+    <t>U0022</t>
+  </si>
+  <si>
+    <t>U0023</t>
+  </si>
+  <si>
+    <t>U0024</t>
+  </si>
+  <si>
+    <t>U0025</t>
+  </si>
+  <si>
+    <t>Tail Gunner</t>
+  </si>
+  <si>
+    <t>When attacking from your rear-facing auxiliary firing arc, reduce the defender's aagility by 1 (to a minimum of '0').</t>
+  </si>
+  <si>
+    <t>Crew</t>
+  </si>
+  <si>
+    <t>Kyle Katarn</t>
+  </si>
+  <si>
+    <t>REBEL ONLY. After you remove a stress token from your ship, you may assign a focus token to your ship.</t>
+  </si>
+  <si>
+    <t>Recon Specialist</t>
+  </si>
+  <si>
+    <t>When you perform a focus action, assign 1 additional focus token to your ship.</t>
+  </si>
+  <si>
+    <t>Systems Officer</t>
+  </si>
+  <si>
+    <t>IMPERIAL ONLY. After you execute a green maneuver, choose another friendly ship at range 1. That ship may acquire a target lock.</t>
+  </si>
+  <si>
+    <t>4-LOM</t>
+  </si>
+  <si>
+    <t>SCUM ONLY. When attacking, during the 'Modify Attack Dice' step, you may receive 1 ion token to choose 1 of the defender's focus or evade tokens. That token cannot be spent during this attack.</t>
+  </si>
+  <si>
+    <t>Zuckuss</t>
+  </si>
+  <si>
+    <t>SCUM ONLY. When attacking, you may receive any number of stress tokens to choose an equal number of defense dice. The defender must reroll those dice.</t>
+  </si>
+  <si>
+    <t>SCUM ONLY. After you perform an attack that does not hit, if you are not stressed, you MUST receive 1 stress token. Then assign 1 focus token to your ship, and acquire a target lock on the defender.</t>
+  </si>
+  <si>
+    <t>Outlaw Tech</t>
+  </si>
+  <si>
+    <t>SCUM ONLY. After you execute a red maneuver, you may assign 1 focus token to your ship.</t>
+  </si>
+  <si>
+    <t>K4 Security Droid</t>
+  </si>
+  <si>
+    <t>SCUM ONLY. After executing a green maneuver, you may acquire a target lock.</t>
+  </si>
+  <si>
+    <t>Greedo</t>
+  </si>
+  <si>
+    <t>SCUM ONLY. The first time you attack each round and the first time you defend each round, the first Damage card dealt is dealt faceup.</t>
+  </si>
+  <si>
+    <t>Jan Ors</t>
+  </si>
+  <si>
+    <t>REBEL ONLY. Once per round, when a friendly ship at Range 1-3 performs a focus action or would be assigned a focus token, you may assign that ship an evade token instead.</t>
+  </si>
+  <si>
+    <t>U0026</t>
+  </si>
+  <si>
+    <t>U0027</t>
+  </si>
+  <si>
+    <t>U0028</t>
+  </si>
+  <si>
+    <t>U0029</t>
+  </si>
+  <si>
+    <t>U0030</t>
+  </si>
+  <si>
+    <t>U0031</t>
+  </si>
+  <si>
+    <t>U0032</t>
+  </si>
+  <si>
+    <t>U0033</t>
+  </si>
+  <si>
+    <t>U0034</t>
+  </si>
+  <si>
+    <t>U0035</t>
+  </si>
+  <si>
+    <t>U0036</t>
+  </si>
+  <si>
+    <t>At the start of the Combat phase, you may discard this card and receive 1 stress token. If you do, until the end of the round, when attacking or defending, you may change all your FOCUS results to HIT or EVADE results.</t>
+  </si>
+  <si>
+    <t>Cloaking Device</t>
+  </si>
+  <si>
+    <t>SMALL SHIP ONLY. ACTION: Perform a free cloak action. At the end of each round, if you are cloaked, roll 1 attack die. On a FOCUS result, discard this card, then decloak or discard your cloak token.</t>
+  </si>
+  <si>
+    <t>Hot-Shot Blaster</t>
+  </si>
+  <si>
+    <t>FP: 3, Rng: 1-2. ATTACK: Discard this card to attack 1 ship (even a ship outside your firing arc).</t>
+  </si>
+  <si>
+    <t>Integrated Astromech</t>
+  </si>
+  <si>
+    <t>X-WING ONLY. When you are dealt a Damage card, you may discard 1 of your ASTROMECH Upgrade cards to discard that Damage card (without resolving its effect).</t>
+  </si>
+  <si>
+    <t>SMALL SHIP ONLY. Your action bar gains the BARREL ROLL action icon.</t>
+  </si>
+  <si>
+    <t>Engine Upgrade</t>
+  </si>
+  <si>
+    <t>Your action bar gains the BOOST action icon.</t>
+  </si>
+  <si>
+    <t>Lightweight Frame</t>
+  </si>
+  <si>
+    <t>TIE ONLY. When defending, after rolling defense dice, if there are more attack dice than there are defense dice, roll 1 additional defence die. You cannot equip this card if your agility value is '3' or higher.</t>
+  </si>
+  <si>
+    <t>Long-Range Scanners</t>
+  </si>
+  <si>
+    <t>You can acquire target locks on ships at range 3 and beyond. You cannot acquire target locks on ships at range 1-2. You can equip this card only if you have TORPEDO and MISSILE in your upgrade bar.</t>
+  </si>
+  <si>
+    <t>B-Wing/E2</t>
+  </si>
+  <si>
+    <t>B-WING ONLY. Your upgrade bar gains the CREW icon.</t>
+  </si>
+  <si>
+    <t>Ion Projector</t>
+  </si>
+  <si>
+    <t>LARGE SHIP ONLY. After an enemy ship executes a maneuver that causes it to overlap your ship, roll 1 attack die. On a HIT or CRIT result, the enemy ship receives 1 ion token.</t>
+  </si>
+  <si>
+    <t>YV-666 ONLY. When you reveal a turn maneuver, you may rotate your dial to the corresponding bank maneuver of the same speed.</t>
+  </si>
+  <si>
+    <t>Maneuvering Finns</t>
+  </si>
+  <si>
+    <t>U0037</t>
+  </si>
+  <si>
+    <t>U0038</t>
+  </si>
+  <si>
+    <t>U0039</t>
+  </si>
+  <si>
+    <t>U0040</t>
+  </si>
+  <si>
+    <t>U0041</t>
+  </si>
+  <si>
+    <t>U0042</t>
+  </si>
+  <si>
+    <t>U0043</t>
+  </si>
+  <si>
+    <t>U0044</t>
+  </si>
+  <si>
+    <t>U0045</t>
+  </si>
+  <si>
+    <t>U0046</t>
+  </si>
+  <si>
+    <t>U0047</t>
+  </si>
+  <si>
+    <t>When attacking or defending, if you are stressed, you may reroll 1 or more of your FOCUS results.</t>
+  </si>
+  <si>
+    <t>Stay On Target</t>
+  </si>
+  <si>
+    <t>When you reveal a meneuver, you may rotate your dial to another maneuver with the same speed. Treat your maneuver as a red maneuver.</t>
+  </si>
+  <si>
+    <t>Cool Hand</t>
+  </si>
+  <si>
+    <t>When you receive a stress token, you may discard this card to assign 1 focus or evade token to your ship.</t>
+  </si>
+  <si>
+    <t>Swarm Leader</t>
+  </si>
+  <si>
+    <t>When performing a primary weapon attack, choose up to 2 other friendly ships that have the defender inside their firing arcs at range 1-3. Remove 1 evade token from each chosen ship to roll 1 additional attack die for every token removed.</t>
+  </si>
+  <si>
+    <t>Adrenaline Rush</t>
+  </si>
+  <si>
+    <t>When you reveal a red maneuver, you may discard this card to treat that maneuver as a white maneuver until the end of the Activation Phase</t>
+  </si>
+  <si>
+    <t>Adaptability</t>
+  </si>
+  <si>
+    <t>DUAL CARD. Increase your pilot skill value by 1. / Decrease your pilot skill value by 1.</t>
+  </si>
+  <si>
+    <t>Lone Wolf</t>
+  </si>
+  <si>
+    <t>When attacking or defending, if there are no other friendly ships at range 1-2, you may reroll 1 of your blank results.</t>
+  </si>
+  <si>
+    <t>Crack Shot</t>
+  </si>
+  <si>
+    <t>When attacking a ship inside your firing arc, you may discard this card to cancel 1 of the defender's EVADE results.</t>
+  </si>
+  <si>
+    <t>Fearlessness</t>
+  </si>
+  <si>
+    <t>SCUM ONLY. When attacking, if you are inside of the defender's firing arc at Range 1 and the defender is inside your firing arc, you may add 1 HIT to your roll.</t>
+  </si>
+  <si>
+    <t>Juke</t>
+  </si>
+  <si>
+    <t>SMALL SHIP ONLY. When attacking, if you have an evade token, you may change one of the defender's EVADE results to a FOCUS result.</t>
+  </si>
+  <si>
+    <t>U0048</t>
+  </si>
+  <si>
+    <t>U0049</t>
+  </si>
+  <si>
+    <t>U0050</t>
+  </si>
+  <si>
+    <t>U0051</t>
+  </si>
+  <si>
+    <t>U0052</t>
+  </si>
+  <si>
+    <t>U0053</t>
+  </si>
+  <si>
+    <t>U0054</t>
+  </si>
+  <si>
+    <t>U0055</t>
+  </si>
+  <si>
+    <t>U0056</t>
+  </si>
+  <si>
+    <t>U0057</t>
+  </si>
+  <si>
+    <t>U0058</t>
+  </si>
+  <si>
+    <t>U0059</t>
+  </si>
+  <si>
+    <t>U0060</t>
+  </si>
+  <si>
+    <t>U0061</t>
+  </si>
+  <si>
+    <t>U0062</t>
+  </si>
+  <si>
+    <t>U0063</t>
+  </si>
+  <si>
+    <t>U0064</t>
+  </si>
+  <si>
+    <t>Autoblaster Turret</t>
+  </si>
+  <si>
+    <t>FP: 2, RNG: 1 ATTACK: Attack 1 ship (even outside your firing arc). Your HIT results cannot be canceled by defense dice. The defender may cancel CRIT results before HIT results.</t>
+  </si>
+  <si>
+    <t>Turret</t>
+  </si>
+  <si>
+    <t>Ion Cannon</t>
+  </si>
+  <si>
+    <t>FP: 3, RNG 1-3 ATTACK: Attack 1 ship. If this attack hits, the defender suffers 1 damage and receives 1 ion token. Then cancel ALL dice results.</t>
+  </si>
+  <si>
+    <t>Cannon</t>
+  </si>
+  <si>
+    <t>Heavy Laser Cannon</t>
+  </si>
+  <si>
+    <t>FP: 4, RNG: 2-3 ATTACK: Attack 1 ship. Immediately after rolling your attack dice, you must cahnge all of your CRIT results to HIT results.</t>
+  </si>
+  <si>
+    <t>Autoblaster</t>
+  </si>
+  <si>
+    <t>FP: 3, RNG 1 ATTACK: Attack 1 ship. Your HIT results cannot be cancelled by defense dice. The defender may cancel CRIT results before HIT results.</t>
+  </si>
+  <si>
+    <t>Tractor Beam</t>
+  </si>
+  <si>
+    <t>FP: 3, RNG 1-3 ATTACK: Attack 1 ship. If this attack hits, the defender receives 1 tractor beam token. Then cancel ALL dice results.</t>
+  </si>
+  <si>
+    <t>Cluster Mines</t>
+  </si>
+  <si>
+    <t>ACTION: Discard this card to DROP 1 cluster mine token set. When a ships base or maneuver template overlaps a cluster mine token, that token DETONATES.</t>
+  </si>
+  <si>
+    <t>Bomb</t>
+  </si>
+  <si>
+    <t>Proximity Mines</t>
+  </si>
+  <si>
+    <t>ACTION: Discard this card to DROP 1 Proximity Mine token. When a ships base or maneuver template overlaps this token, the token detonates.</t>
+  </si>
+  <si>
+    <t>Chardaan Refit</t>
+  </si>
+  <si>
+    <t>A-WING ONLY. This card has a negative squad point cost.</t>
+  </si>
+  <si>
+    <t>Missile</t>
+  </si>
+  <si>
+    <t>Proton Rockers</t>
+  </si>
+  <si>
+    <t>FP: 2, RNG 1 ATTACK (FOCUS): Discard thsi card to perform this attack. You may roll additional dice equal to your agility value, up to a maximum of 3 additional dice.</t>
+  </si>
+  <si>
+    <t>Seismic Torpedo</t>
+  </si>
+  <si>
+    <t>ACTION: Discard this car to choose an obstacle at range 1-2 and inside your primary firing arc. Each ship at range 1 of the obstacle rolls 1 attack die and suffers any HIT or CRIT rolled. Then remove the obstacle.</t>
+  </si>
+  <si>
+    <t>Torpedo</t>
+  </si>
+  <si>
+    <t>Adv. Proton Torpedoes</t>
+  </si>
+  <si>
+    <t>FP: 5, RNG 1 ATTACK (TARGET LOCK): Spend your target lock and discard this card to perform this attack. You may change up to 3 of your blank results to FOCUS results.</t>
+  </si>
+  <si>
+    <t>Proton Torpedoes</t>
+  </si>
+  <si>
+    <t>FP: 4, RNG 2-3 ATTACK (TARGET LOCK): Spend your target lock and discard this card to make the attack. You may change one of your FOCUS results to a CRIT result.</t>
+  </si>
+  <si>
+    <t>Bomb Loadout</t>
+  </si>
+  <si>
+    <t>Y-WING ONLY. Your upgrade bar gains the BOMB upgrade icon.</t>
+  </si>
+  <si>
+    <t>U0065</t>
+  </si>
+  <si>
+    <t>U0066</t>
+  </si>
+  <si>
+    <t>U0067</t>
+  </si>
+  <si>
+    <t>U0068</t>
+  </si>
+  <si>
+    <t>U0069</t>
+  </si>
+  <si>
+    <t>U0070</t>
   </si>
 </sst>
 </file>
@@ -264,9 +885,27 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -594,7 +1233,7 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>0</v>
@@ -605,7 +1244,7 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>55</v>
+        <v>50</v>
       </c>
       <c r="B2" t="s">
         <v>6</v>
@@ -616,7 +1255,7 @@
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>56</v>
+        <v>51</v>
       </c>
       <c r="B3" t="s">
         <v>7</v>
@@ -627,7 +1266,7 @@
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>57</v>
+        <v>52</v>
       </c>
       <c r="B4" t="s">
         <v>8</v>
@@ -638,7 +1277,7 @@
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>58</v>
+        <v>53</v>
       </c>
       <c r="B5" t="s">
         <v>9</v>
@@ -649,7 +1288,7 @@
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>59</v>
+        <v>54</v>
       </c>
       <c r="B6" t="s">
         <v>10</v>
@@ -660,7 +1299,7 @@
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>60</v>
+        <v>55</v>
       </c>
       <c r="B7" t="s">
         <v>11</v>
@@ -671,7 +1310,7 @@
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>61</v>
+        <v>56</v>
       </c>
       <c r="B8" t="s">
         <v>12</v>
@@ -682,7 +1321,7 @@
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>62</v>
+        <v>57</v>
       </c>
       <c r="B9" t="s">
         <v>13</v>
@@ -693,7 +1332,7 @@
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>63</v>
+        <v>58</v>
       </c>
       <c r="B10" t="s">
         <v>14</v>
@@ -704,7 +1343,7 @@
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>64</v>
+        <v>59</v>
       </c>
       <c r="B11" t="s">
         <v>15</v>
@@ -735,19 +1374,19 @@
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>2</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="F1" s="1" t="s">
         <v>0</v>
@@ -756,19 +1395,19 @@
         <v>5</v>
       </c>
       <c r="H1" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="I1" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="K1" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="L1" s="1" t="s">
         <v>41</v>
-      </c>
-      <c r="L1" s="1" t="s">
-        <v>42</v>
       </c>
       <c r="M1" s="1" t="s">
         <v>1</v>
@@ -776,22 +1415,22 @@
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B2" t="s">
         <v>16</v>
       </c>
       <c r="C2" t="s">
+        <v>27</v>
+      </c>
+      <c r="D2">
+        <v>30</v>
+      </c>
+      <c r="E2" t="s">
+        <v>29</v>
+      </c>
+      <c r="F2" t="s">
         <v>28</v>
-      </c>
-      <c r="D2">
-        <v>30</v>
-      </c>
-      <c r="E2" t="s">
-        <v>30</v>
-      </c>
-      <c r="F2" t="s">
-        <v>29</v>
       </c>
       <c r="G2" t="s">
         <v>17</v>
@@ -817,19 +1456,19 @@
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B3" t="s">
+        <v>31</v>
+      </c>
+      <c r="C3" t="s">
         <v>32</v>
-      </c>
-      <c r="C3" t="s">
-        <v>33</v>
       </c>
       <c r="D3">
         <v>33</v>
       </c>
       <c r="E3" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="F3" t="s">
         <v>13</v>
@@ -858,25 +1497,25 @@
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B4" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C4" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D4">
         <v>15</v>
       </c>
       <c r="E4" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="F4" t="s">
         <v>7</v>
       </c>
       <c r="G4" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="H4">
         <v>2</v>
@@ -905,142 +1544,1865 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{18EF0634-2CFE-451C-B280-271F73D0B3E3}">
-  <dimension ref="A1:H5"/>
+  <dimension ref="A1:H71"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H6" sqref="H6"/>
+      <pane ySplit="1" topLeftCell="A58" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A63" sqref="A63:A71"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="7.44140625" customWidth="1"/>
+    <col min="2" max="2" width="21.109375" customWidth="1"/>
+    <col min="3" max="3" width="126.77734375" style="2" customWidth="1"/>
+    <col min="7" max="7" width="13.21875" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A1" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="C1" s="1" t="s">
+      <c r="A1" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="F1" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="G1" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="H1" s="3" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A2" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="B2" s="5" t="s">
+        <v>60</v>
+      </c>
+      <c r="C2" s="6" t="s">
+        <v>63</v>
+      </c>
+      <c r="D2" s="5">
+        <v>0</v>
+      </c>
+      <c r="E2" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="F2" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="G2" s="5" t="s">
+        <v>61</v>
+      </c>
+      <c r="H2" s="5">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A3" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="B3" s="5" t="s">
+        <v>62</v>
+      </c>
+      <c r="C3" s="6" t="s">
+        <v>64</v>
+      </c>
+      <c r="D3" s="5">
+        <v>0</v>
+      </c>
+      <c r="E3" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="F3" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="G3" s="5" t="s">
+        <v>61</v>
+      </c>
+      <c r="H3" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A4" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="B4" s="5" t="s">
+        <v>65</v>
+      </c>
+      <c r="C4" s="6" t="s">
+        <v>66</v>
+      </c>
+      <c r="D4" s="5">
+        <v>0</v>
+      </c>
+      <c r="E4" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="F4" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="G4" s="5" t="s">
+        <v>61</v>
+      </c>
+      <c r="H4" s="5">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A5" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="B5" s="5" t="s">
+        <v>67</v>
+      </c>
+      <c r="C5" s="6" t="s">
+        <v>82</v>
+      </c>
+      <c r="D5" s="5">
+        <v>-2</v>
+      </c>
+      <c r="E5" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="F5" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="G5" s="5" t="s">
+        <v>61</v>
+      </c>
+      <c r="H5" s="5">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A6" s="5" t="s">
+        <v>84</v>
+      </c>
+      <c r="B6" s="5" t="s">
+        <v>68</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="D6" s="5">
+        <v>0</v>
+      </c>
+      <c r="E6" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="F6" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="G6" s="5" t="s">
+        <v>61</v>
+      </c>
+      <c r="H6" s="5">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A7" s="5" t="s">
+        <v>85</v>
+      </c>
+      <c r="B7" s="5" t="s">
+        <v>70</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="D7" s="5">
+        <v>0</v>
+      </c>
+      <c r="E7" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="F7" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="G7" s="5" t="s">
+        <v>61</v>
+      </c>
+      <c r="H7" s="5">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A8" s="5" t="s">
+        <v>86</v>
+      </c>
+      <c r="B8" s="5" t="s">
+        <v>71</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="D8" s="5">
+        <v>0</v>
+      </c>
+      <c r="E8" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="F8" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="G8" s="5" t="s">
+        <v>61</v>
+      </c>
+      <c r="H8" s="5">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A9" s="5" t="s">
+        <v>87</v>
+      </c>
+      <c r="B9" s="5" t="s">
+        <v>73</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="D9" s="5">
+        <v>0</v>
+      </c>
+      <c r="E9" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="F9" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="G9" s="5" t="s">
+        <v>61</v>
+      </c>
+      <c r="H9" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A10" s="5" t="s">
+        <v>88</v>
+      </c>
+      <c r="B10" s="5" t="s">
+        <v>75</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="D10" s="5">
+        <v>6</v>
+      </c>
+      <c r="E10" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="F10" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="G10" s="5" t="s">
+        <v>61</v>
+      </c>
+      <c r="H10" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A11" s="5" t="s">
+        <v>89</v>
+      </c>
+      <c r="B11" s="5" t="s">
+        <v>77</v>
+      </c>
+      <c r="C11" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="D11" s="5">
+        <v>0</v>
+      </c>
+      <c r="E11" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="F11" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="G11" s="5" t="s">
+        <v>61</v>
+      </c>
+      <c r="H11" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A12" s="5" t="s">
+        <v>90</v>
+      </c>
+      <c r="B12" s="5" t="s">
+        <v>79</v>
+      </c>
+      <c r="C12" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="D12" s="5">
+        <v>1</v>
+      </c>
+      <c r="E12" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="F12" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="G12" s="5" t="s">
+        <v>61</v>
+      </c>
+      <c r="H12" s="5">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A13" s="5" t="s">
+        <v>121</v>
+      </c>
+      <c r="B13" s="5" t="s">
+        <v>91</v>
+      </c>
+      <c r="C13" s="2" t="s">
+        <v>92</v>
+      </c>
+      <c r="D13" s="5">
+        <v>2</v>
+      </c>
+      <c r="E13" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="F13" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="G13" s="5" t="s">
+        <v>83</v>
+      </c>
+      <c r="H13" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A14" s="5" t="s">
+        <v>122</v>
+      </c>
+      <c r="B14" s="5" t="s">
+        <v>93</v>
+      </c>
+      <c r="C14" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="D14" s="5">
+        <v>1</v>
+      </c>
+      <c r="E14" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="F14" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="G14" s="5" t="s">
+        <v>83</v>
+      </c>
+      <c r="H14" s="5">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A15" s="5" t="s">
+        <v>123</v>
+      </c>
+      <c r="B15" s="5" t="s">
+        <v>95</v>
+      </c>
+      <c r="C15" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="D15" s="5">
+        <v>1</v>
+      </c>
+      <c r="E15" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="F15" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="G15" s="5" t="s">
+        <v>83</v>
+      </c>
+      <c r="H15" s="5">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A16" s="5" t="s">
+        <v>124</v>
+      </c>
+      <c r="B16" s="5" t="s">
+        <v>97</v>
+      </c>
+      <c r="C16" s="2" t="s">
+        <v>98</v>
+      </c>
+      <c r="D16" s="5">
+        <v>2</v>
+      </c>
+      <c r="E16" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="F16" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="G16" s="5" t="s">
+        <v>99</v>
+      </c>
+      <c r="H16" s="5">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A17" s="5" t="s">
+        <v>125</v>
+      </c>
+      <c r="B17" s="5" t="s">
+        <v>100</v>
+      </c>
+      <c r="C17" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="D17" s="5">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="G1" s="1" t="s">
+      <c r="E17" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="F17" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="G17" s="5" t="s">
+        <v>99</v>
+      </c>
+      <c r="H17" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A18" s="5" t="s">
+        <v>126</v>
+      </c>
+      <c r="B18" s="5" t="s">
+        <v>102</v>
+      </c>
+      <c r="C18" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="D18" s="5">
+        <v>2</v>
+      </c>
+      <c r="E18" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="F18" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="G18" s="5" t="s">
+        <v>104</v>
+      </c>
+      <c r="H18" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A19" s="5" t="s">
+        <v>127</v>
+      </c>
+      <c r="B19" s="5" t="s">
+        <v>105</v>
+      </c>
+      <c r="C19" s="2" t="s">
+        <v>106</v>
+      </c>
+      <c r="D19" s="5">
+        <v>2</v>
+      </c>
+      <c r="E19" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="F19" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="G19" s="5" t="s">
+        <v>104</v>
+      </c>
+      <c r="H19" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A20" s="5" t="s">
+        <v>128</v>
+      </c>
+      <c r="B20" s="5" t="s">
+        <v>107</v>
+      </c>
+      <c r="C20" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="D20" s="5">
+        <v>1</v>
+      </c>
+      <c r="E20" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="F20" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="G20" s="5" t="s">
+        <v>104</v>
+      </c>
+      <c r="H20" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A21" s="5" t="s">
+        <v>129</v>
+      </c>
+      <c r="B21" s="5" t="s">
+        <v>109</v>
+      </c>
+      <c r="C21" s="2" t="s">
+        <v>110</v>
+      </c>
+      <c r="D21" s="5">
+        <v>2</v>
+      </c>
+      <c r="E21" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="F21" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="G21" s="5" t="s">
+        <v>104</v>
+      </c>
+      <c r="H21" s="5">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A22" s="5" t="s">
+        <v>130</v>
+      </c>
+      <c r="B22" s="5" t="s">
+        <v>111</v>
+      </c>
+      <c r="C22" s="2" t="s">
+        <v>112</v>
+      </c>
+      <c r="D22" s="5">
+        <v>2</v>
+      </c>
+      <c r="E22" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="F22" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="G22" s="5" t="s">
+        <v>113</v>
+      </c>
+      <c r="H22" s="5">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A23" s="5" t="s">
+        <v>131</v>
+      </c>
+      <c r="B23" s="5" t="s">
+        <v>114</v>
+      </c>
+      <c r="C23" s="2" t="s">
+        <v>115</v>
+      </c>
+      <c r="D23" s="5">
+        <v>3</v>
+      </c>
+      <c r="E23" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="F23" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="G23" s="5" t="s">
+        <v>113</v>
+      </c>
+      <c r="H23" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A24" s="5" t="s">
+        <v>132</v>
+      </c>
+      <c r="B24" s="7" t="s">
+        <v>116</v>
+      </c>
+      <c r="C24" s="2" t="s">
+        <v>117</v>
+      </c>
+      <c r="D24" s="5">
+        <v>0</v>
+      </c>
+      <c r="E24" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="F24" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="G24" s="5" t="s">
+        <v>113</v>
+      </c>
+      <c r="H24" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A25" s="5" t="s">
+        <v>133</v>
+      </c>
+      <c r="B25" s="5" t="s">
+        <v>113</v>
+      </c>
+      <c r="C25" s="2" t="s">
+        <v>118</v>
+      </c>
+      <c r="D25" s="5">
+        <v>2</v>
+      </c>
+      <c r="E25" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="F25" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="G25" s="5" t="s">
+        <v>113</v>
+      </c>
+      <c r="H25" s="5">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A26" s="5" t="s">
+        <v>134</v>
+      </c>
+      <c r="B26" s="5" t="s">
+        <v>119</v>
+      </c>
+      <c r="C26" s="2" t="s">
+        <v>120</v>
+      </c>
+      <c r="D26" s="5">
+        <v>1</v>
+      </c>
+      <c r="E26" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="F26" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="G26" s="5" t="s">
+        <v>113</v>
+      </c>
+      <c r="H26" s="5">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A27" s="5" t="s">
+        <v>157</v>
+      </c>
+      <c r="B27" s="5" t="s">
+        <v>135</v>
+      </c>
+      <c r="C27" s="2" t="s">
+        <v>136</v>
+      </c>
+      <c r="D27" s="5">
+        <v>2</v>
+      </c>
+      <c r="E27" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="F27" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="G27" s="5" t="s">
+        <v>137</v>
+      </c>
+      <c r="H27" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A28" s="5" t="s">
+        <v>158</v>
+      </c>
+      <c r="B28" s="5" t="s">
+        <v>138</v>
+      </c>
+      <c r="C28" s="2" t="s">
+        <v>139</v>
+      </c>
+      <c r="D28" s="5">
+        <v>3</v>
+      </c>
+      <c r="E28" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="F28" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="G28" s="5" t="s">
+        <v>137</v>
+      </c>
+      <c r="H28" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A29" s="5" t="s">
+        <v>159</v>
+      </c>
+      <c r="B29" s="5" t="s">
+        <v>140</v>
+      </c>
+      <c r="C29" s="2" t="s">
+        <v>141</v>
+      </c>
+      <c r="D29" s="5">
+        <v>3</v>
+      </c>
+      <c r="E29" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="F29" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="G29" s="5" t="s">
+        <v>137</v>
+      </c>
+      <c r="H29" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="30" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A30" s="5" t="s">
+        <v>160</v>
+      </c>
+      <c r="B30" s="5" t="s">
+        <v>142</v>
+      </c>
+      <c r="C30" s="2" t="s">
+        <v>143</v>
+      </c>
+      <c r="D30" s="5">
+        <v>2</v>
+      </c>
+      <c r="E30" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="F30" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="G30" s="5" t="s">
+        <v>137</v>
+      </c>
+      <c r="H30" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="31" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A31" s="5" t="s">
+        <v>161</v>
+      </c>
+      <c r="B31" s="5" t="s">
+        <v>144</v>
+      </c>
+      <c r="C31" s="2" t="s">
+        <v>145</v>
+      </c>
+      <c r="D31" s="5">
+        <v>1</v>
+      </c>
+      <c r="E31" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="F31" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="G31" s="5" t="s">
+        <v>137</v>
+      </c>
+      <c r="H31" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="32" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A32" s="5" t="s">
+        <v>162</v>
+      </c>
+      <c r="B32" s="5" t="s">
+        <v>146</v>
+      </c>
+      <c r="C32" s="2" t="s">
+        <v>147</v>
+      </c>
+      <c r="D32" s="5">
+        <v>1</v>
+      </c>
+      <c r="E32" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="F32" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="G32" s="5" t="s">
+        <v>137</v>
+      </c>
+      <c r="H32" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="33" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A33" s="5" t="s">
+        <v>163</v>
+      </c>
+      <c r="B33" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="C33" s="2" t="s">
+        <v>148</v>
+      </c>
+      <c r="D33" s="5">
+        <v>2</v>
+      </c>
+      <c r="E33" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="F33" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="G33" s="5" t="s">
+        <v>137</v>
+      </c>
+      <c r="H33" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="34" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A34" s="5" t="s">
+        <v>164</v>
+      </c>
+      <c r="B34" s="5" t="s">
+        <v>149</v>
+      </c>
+      <c r="C34" s="2" t="s">
+        <v>150</v>
+      </c>
+      <c r="D34" s="5">
+        <v>2</v>
+      </c>
+      <c r="E34" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="F34" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="G34" s="5" t="s">
+        <v>137</v>
+      </c>
+      <c r="H34" s="5">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="35" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A35" s="5" t="s">
+        <v>165</v>
+      </c>
+      <c r="B35" s="5" t="s">
+        <v>151</v>
+      </c>
+      <c r="C35" s="2" t="s">
+        <v>152</v>
+      </c>
+      <c r="D35" s="5">
+        <v>3</v>
+      </c>
+      <c r="E35" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="F35" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="G35" s="5" t="s">
+        <v>137</v>
+      </c>
+      <c r="H35" s="5">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="36" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A36" s="5" t="s">
+        <v>166</v>
+      </c>
+      <c r="B36" s="5" t="s">
+        <v>153</v>
+      </c>
+      <c r="C36" s="2" t="s">
+        <v>154</v>
+      </c>
+      <c r="D36" s="5">
+        <v>1</v>
+      </c>
+      <c r="E36" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="F36" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="G36" s="5" t="s">
+        <v>137</v>
+      </c>
+      <c r="H36" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="37" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A37" s="5" t="s">
+        <v>167</v>
+      </c>
+      <c r="B37" s="5" t="s">
+        <v>155</v>
+      </c>
+      <c r="C37" s="2" t="s">
+        <v>156</v>
+      </c>
+      <c r="D37" s="5">
+        <v>2</v>
+      </c>
+      <c r="E37" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="F37" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="G37" s="5" t="s">
+        <v>137</v>
+      </c>
+      <c r="H37" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="38" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A38" s="5" t="s">
+        <v>188</v>
+      </c>
+      <c r="B38" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="C38" s="2" t="s">
+        <v>168</v>
+      </c>
+      <c r="D38" s="5">
+        <v>2</v>
+      </c>
+      <c r="E38" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="F38" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="G38" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="H38" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="39" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A39" s="5" t="s">
+        <v>189</v>
+      </c>
+      <c r="B39" s="5" t="s">
+        <v>169</v>
+      </c>
+      <c r="C39" s="2" t="s">
+        <v>170</v>
+      </c>
+      <c r="D39" s="5">
+        <v>2</v>
+      </c>
+      <c r="E39" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="F39" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="G39" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="H39" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="40" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A40" s="5" t="s">
+        <v>190</v>
+      </c>
+      <c r="B40" s="5" t="s">
+        <v>171</v>
+      </c>
+      <c r="C40" s="2" t="s">
+        <v>172</v>
+      </c>
+      <c r="D40" s="5">
+        <v>3</v>
+      </c>
+      <c r="E40" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="F40" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="G40" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="H40" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="41" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A41" s="5" t="s">
+        <v>191</v>
+      </c>
+      <c r="B41" s="5" t="s">
+        <v>173</v>
+      </c>
+      <c r="C41" s="2" t="s">
+        <v>174</v>
+      </c>
+      <c r="D41" s="5">
+        <v>0</v>
+      </c>
+      <c r="E41" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="F41" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="G41" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="H41" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="42" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A42" s="5" t="s">
+        <v>192</v>
+      </c>
+      <c r="B42" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="C42" s="2" t="s">
+        <v>175</v>
+      </c>
+      <c r="D42" s="5">
+        <v>2</v>
+      </c>
+      <c r="E42" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="F42" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="G42" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="H42" s="5">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="43" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A43" s="5" t="s">
+        <v>193</v>
+      </c>
+      <c r="B43" s="5" t="s">
+        <v>176</v>
+      </c>
+      <c r="C43" s="2" t="s">
+        <v>177</v>
+      </c>
+      <c r="D43" s="5">
         <v>4</v>
       </c>
-      <c r="H1" s="1" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
-        <v>46</v>
-      </c>
-      <c r="B2" t="s">
+      <c r="E43" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="F43" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="G43" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="H43" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="44" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A44" s="5" t="s">
+        <v>194</v>
+      </c>
+      <c r="B44" s="5" t="s">
+        <v>178</v>
+      </c>
+      <c r="C44" s="2" t="s">
+        <v>179</v>
+      </c>
+      <c r="D44" s="5">
+        <v>2</v>
+      </c>
+      <c r="E44" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="F44" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="G44" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="H44" s="5">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="45" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A45" s="5" t="s">
+        <v>195</v>
+      </c>
+      <c r="B45" s="5" t="s">
+        <v>180</v>
+      </c>
+      <c r="C45" s="2" t="s">
+        <v>181</v>
+      </c>
+      <c r="D45" s="5">
+        <v>0</v>
+      </c>
+      <c r="E45" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="F45" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="G45" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="H45" s="5">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="46" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A46" s="5" t="s">
+        <v>196</v>
+      </c>
+      <c r="B46" s="5" t="s">
+        <v>182</v>
+      </c>
+      <c r="C46" s="2" t="s">
+        <v>183</v>
+      </c>
+      <c r="D46" s="5">
+        <v>1</v>
+      </c>
+      <c r="E46" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="F46" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="G46" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="H46" s="5">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="47" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A47" s="5" t="s">
+        <v>197</v>
+      </c>
+      <c r="B47" s="5" t="s">
+        <v>184</v>
+      </c>
+      <c r="C47" s="2" t="s">
+        <v>185</v>
+      </c>
+      <c r="D47" s="5">
+        <v>2</v>
+      </c>
+      <c r="E47" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="F47" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="G47" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="H47" s="5">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="48" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A48" s="5" t="s">
+        <v>198</v>
+      </c>
+      <c r="B48" s="5" t="s">
+        <v>187</v>
+      </c>
+      <c r="C48" s="2" t="s">
+        <v>186</v>
+      </c>
+      <c r="D48" s="5">
+        <v>1</v>
+      </c>
+      <c r="E48" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="F48" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="G48" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="H48" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="49" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A49" s="5" t="s">
+        <v>218</v>
+      </c>
+      <c r="B49" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="C2" t="s">
-        <v>51</v>
-      </c>
-      <c r="D2">
-        <v>1</v>
-      </c>
-      <c r="E2" t="s">
-        <v>31</v>
-      </c>
-      <c r="F2" t="s">
-        <v>31</v>
-      </c>
-      <c r="G2" t="s">
+      <c r="C49" s="2" t="s">
+        <v>199</v>
+      </c>
+      <c r="D49" s="5">
+        <v>1</v>
+      </c>
+      <c r="E49" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="F49" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="G49" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="H2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
-        <v>47</v>
-      </c>
-      <c r="B3" t="s">
-        <v>21</v>
-      </c>
-      <c r="C3" t="s">
-        <v>52</v>
-      </c>
-      <c r="D3">
-        <v>1</v>
-      </c>
-      <c r="E3" t="s">
-        <v>31</v>
-      </c>
-      <c r="F3" t="s">
-        <v>31</v>
-      </c>
-      <c r="G3" t="s">
+      <c r="H49" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="50" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A50" s="5" t="s">
+        <v>219</v>
+      </c>
+      <c r="B50" s="5" t="s">
+        <v>200</v>
+      </c>
+      <c r="C50" s="2" t="s">
+        <v>201</v>
+      </c>
+      <c r="D50" s="5">
+        <v>2</v>
+      </c>
+      <c r="E50" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="F50" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="G50" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="H3">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
-        <v>48</v>
-      </c>
-      <c r="B4" t="s">
-        <v>22</v>
-      </c>
-      <c r="C4" t="s">
-        <v>53</v>
-      </c>
-      <c r="D4">
-        <v>2</v>
-      </c>
-      <c r="E4" t="s">
-        <v>31</v>
-      </c>
-      <c r="F4" t="s">
-        <v>30</v>
-      </c>
-      <c r="G4" t="s">
-        <v>23</v>
-      </c>
-      <c r="H4">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A5" t="s">
-        <v>49</v>
-      </c>
-      <c r="B5" t="s">
-        <v>24</v>
-      </c>
-      <c r="C5" t="s">
-        <v>54</v>
-      </c>
-      <c r="D5">
-        <v>2</v>
-      </c>
-      <c r="E5" t="s">
-        <v>31</v>
-      </c>
-      <c r="F5" t="s">
-        <v>31</v>
-      </c>
-      <c r="G5" t="s">
-        <v>25</v>
-      </c>
-      <c r="H5">
-        <v>1</v>
+      <c r="H50" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="51" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A51" s="5" t="s">
+        <v>220</v>
+      </c>
+      <c r="B51" s="5" t="s">
+        <v>202</v>
+      </c>
+      <c r="C51" s="2" t="s">
+        <v>203</v>
+      </c>
+      <c r="D51" s="5">
+        <v>1</v>
+      </c>
+      <c r="E51" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="F51" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="G51" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="H51" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="52" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A52" s="5" t="s">
+        <v>221</v>
+      </c>
+      <c r="B52" s="5" t="s">
+        <v>204</v>
+      </c>
+      <c r="C52" s="2" t="s">
+        <v>205</v>
+      </c>
+      <c r="D52" s="5">
+        <v>3</v>
+      </c>
+      <c r="E52" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="F52" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="G52" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="H52" s="5">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="53" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A53" s="5" t="s">
+        <v>222</v>
+      </c>
+      <c r="B53" s="5" t="s">
+        <v>206</v>
+      </c>
+      <c r="C53" s="2" t="s">
+        <v>207</v>
+      </c>
+      <c r="D53" s="5">
+        <v>1</v>
+      </c>
+      <c r="E53" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="F53" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="G53" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="H53" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="54" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A54" s="5" t="s">
+        <v>223</v>
+      </c>
+      <c r="B54" s="5" t="s">
+        <v>208</v>
+      </c>
+      <c r="C54" s="2" t="s">
+        <v>209</v>
+      </c>
+      <c r="D54" s="5">
+        <v>0</v>
+      </c>
+      <c r="E54" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="F54" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="G54" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="H54" s="5">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="55" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A55" s="5" t="s">
+        <v>224</v>
+      </c>
+      <c r="B55" s="5" t="s">
+        <v>210</v>
+      </c>
+      <c r="C55" s="2" t="s">
+        <v>211</v>
+      </c>
+      <c r="D55" s="5">
+        <v>2</v>
+      </c>
+      <c r="E55" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="F55" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="G55" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="H55" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="56" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A56" s="5" t="s">
+        <v>225</v>
+      </c>
+      <c r="B56" s="5" t="s">
+        <v>212</v>
+      </c>
+      <c r="C56" s="2" t="s">
+        <v>213</v>
+      </c>
+      <c r="D56" s="5">
+        <v>1</v>
+      </c>
+      <c r="E56" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="F56" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="G56" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="H56" s="5">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="57" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A57" s="5" t="s">
+        <v>226</v>
+      </c>
+      <c r="B57" s="5" t="s">
+        <v>214</v>
+      </c>
+      <c r="C57" s="2" t="s">
+        <v>215</v>
+      </c>
+      <c r="D57" s="5">
+        <v>1</v>
+      </c>
+      <c r="E57" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="F57" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="G57" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="H57" s="5">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="58" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A58" s="5" t="s">
+        <v>227</v>
+      </c>
+      <c r="B58" s="5" t="s">
+        <v>216</v>
+      </c>
+      <c r="C58" s="2" t="s">
+        <v>217</v>
+      </c>
+      <c r="D58" s="5">
+        <v>2</v>
+      </c>
+      <c r="E58" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="F58" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="G58" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="H58" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="59" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A59" s="5" t="s">
+        <v>228</v>
+      </c>
+      <c r="B59" s="5" t="s">
+        <v>235</v>
+      </c>
+      <c r="C59" s="2" t="s">
+        <v>236</v>
+      </c>
+      <c r="D59" s="5">
+        <v>2</v>
+      </c>
+      <c r="E59" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="F59" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="G59" s="5" t="s">
+        <v>237</v>
+      </c>
+      <c r="H59" s="5">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="60" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A60" s="5" t="s">
+        <v>229</v>
+      </c>
+      <c r="B60" s="5" t="s">
+        <v>238</v>
+      </c>
+      <c r="C60" s="2" t="s">
+        <v>239</v>
+      </c>
+      <c r="D60" s="5">
+        <v>3</v>
+      </c>
+      <c r="E60" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="F60" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="G60" s="5" t="s">
+        <v>240</v>
+      </c>
+      <c r="H60" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="61" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A61" s="5" t="s">
+        <v>230</v>
+      </c>
+      <c r="B61" s="5" t="s">
+        <v>241</v>
+      </c>
+      <c r="C61" s="2" t="s">
+        <v>242</v>
+      </c>
+      <c r="D61" s="5">
+        <v>7</v>
+      </c>
+      <c r="E61" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="F61" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="G61" s="5" t="s">
+        <v>240</v>
+      </c>
+      <c r="H61" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="62" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A62" s="5" t="s">
+        <v>231</v>
+      </c>
+      <c r="B62" s="5" t="s">
+        <v>243</v>
+      </c>
+      <c r="C62" s="2" t="s">
+        <v>244</v>
+      </c>
+      <c r="D62" s="5">
+        <v>5</v>
+      </c>
+      <c r="E62" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="F62" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="G62" s="5" t="s">
+        <v>240</v>
+      </c>
+      <c r="H62" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="63" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A63" s="5" t="s">
+        <v>232</v>
+      </c>
+      <c r="B63" s="5" t="s">
+        <v>245</v>
+      </c>
+      <c r="C63" s="2" t="s">
+        <v>246</v>
+      </c>
+      <c r="D63" s="5">
+        <v>1</v>
+      </c>
+      <c r="E63" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="F63" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="G63" t="s">
+        <v>240</v>
+      </c>
+      <c r="H63" s="5">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="64" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A64" s="5" t="s">
+        <v>233</v>
+      </c>
+      <c r="B64" s="5" t="s">
+        <v>247</v>
+      </c>
+      <c r="C64" s="2" t="s">
+        <v>248</v>
+      </c>
+      <c r="D64" s="5">
+        <v>4</v>
+      </c>
+      <c r="E64" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="F64" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="G64" s="5" t="s">
+        <v>249</v>
+      </c>
+      <c r="H64" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="65" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A65" s="5" t="s">
+        <v>234</v>
+      </c>
+      <c r="B65" s="5" t="s">
+        <v>250</v>
+      </c>
+      <c r="C65" s="2" t="s">
+        <v>251</v>
+      </c>
+      <c r="D65" s="5">
+        <v>3</v>
+      </c>
+      <c r="E65" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="F65" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="G65" s="5" t="s">
+        <v>249</v>
+      </c>
+      <c r="H65" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="66" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A66" s="5" t="s">
+        <v>266</v>
+      </c>
+      <c r="B66" s="5" t="s">
+        <v>252</v>
+      </c>
+      <c r="C66" s="2" t="s">
+        <v>253</v>
+      </c>
+      <c r="D66" s="5">
+        <v>-2</v>
+      </c>
+      <c r="E66" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="F66" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="G66" s="5" t="s">
+        <v>254</v>
+      </c>
+      <c r="H66" s="5">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="67" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A67" s="5" t="s">
+        <v>267</v>
+      </c>
+      <c r="B67" s="5" t="s">
+        <v>255</v>
+      </c>
+      <c r="C67" s="2" t="s">
+        <v>256</v>
+      </c>
+      <c r="D67" s="5">
+        <v>3</v>
+      </c>
+      <c r="E67" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="F67" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="G67" s="5" t="s">
+        <v>254</v>
+      </c>
+      <c r="H67" s="5">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="68" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A68" s="5" t="s">
+        <v>268</v>
+      </c>
+      <c r="B68" s="5" t="s">
+        <v>257</v>
+      </c>
+      <c r="C68" s="2" t="s">
+        <v>258</v>
+      </c>
+      <c r="D68" s="5">
+        <v>2</v>
+      </c>
+      <c r="E68" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="F68" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="G68" s="5" t="s">
+        <v>259</v>
+      </c>
+      <c r="H68" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="69" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A69" s="5" t="s">
+        <v>269</v>
+      </c>
+      <c r="B69" s="5" t="s">
+        <v>260</v>
+      </c>
+      <c r="C69" s="2" t="s">
+        <v>261</v>
+      </c>
+      <c r="D69" s="5">
+        <v>6</v>
+      </c>
+      <c r="E69" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="F69" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="G69" s="5" t="s">
+        <v>259</v>
+      </c>
+      <c r="H69" s="5">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="70" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A70" s="5" t="s">
+        <v>270</v>
+      </c>
+      <c r="B70" s="5" t="s">
+        <v>262</v>
+      </c>
+      <c r="C70" s="2" t="s">
+        <v>263</v>
+      </c>
+      <c r="D70" s="5">
+        <v>4</v>
+      </c>
+      <c r="E70" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="F70" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="G70" s="5" t="s">
+        <v>259</v>
+      </c>
+      <c r="H70" s="5">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="71" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A71" s="5" t="s">
+        <v>271</v>
+      </c>
+      <c r="B71" s="5" t="s">
+        <v>264</v>
+      </c>
+      <c r="C71" s="2" t="s">
+        <v>265</v>
+      </c>
+      <c r="D71" s="5">
+        <v>0</v>
+      </c>
+      <c r="E71" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="F71" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="G71" s="5" t="s">
+        <v>259</v>
+      </c>
+      <c r="H71" s="5">
+        <v>2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add new Upgrade cards to DB
</commit_message>
<xml_diff>
--- a/VadersLittleHelper/db/ComponentDB.xlsx
+++ b/VadersLittleHelper/db/ComponentDB.xlsx
@@ -1,22 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18326"/>
-  <workbookPr defaultThemeVersion="166925"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Victor Dalqvist\Documents\VadersLittleHelper\VadersLittleHelper\db\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Victor\Documents\VadersLittleHelper\VadersLittleHelper\db\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="5292" windowHeight="5796" activeTab="2" xr2:uid="{EFCB0871-0F77-484A-948E-5B1FEFF48867}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="5295" windowHeight="5790" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="ShipDB" sheetId="1" r:id="rId1"/>
     <sheet name="PilotDB" sheetId="3" r:id="rId2"/>
     <sheet name="CardDB" sheetId="2" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="171027"/>
+  <calcPr calcId="152511"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="482" uniqueCount="272">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="716" uniqueCount="383">
   <si>
     <t>Ship</t>
   </si>
@@ -842,12 +842,345 @@
   </si>
   <si>
     <t>U0070</t>
+  </si>
+  <si>
+    <t>Collision Detector</t>
+  </si>
+  <si>
+    <t>When performing a boost, barrel roll, or decloak, your ship and maneuver template can overlap obstacles. When rolling for obstacle damage, ignore all CRIT results.</t>
+  </si>
+  <si>
+    <t>Sensor Cluster</t>
+  </si>
+  <si>
+    <t>When defending, you may spend a focus token to change one of your blank results to an EVADE result.</t>
+  </si>
+  <si>
+    <t>Special Ops Training</t>
+  </si>
+  <si>
+    <t>TIE/SF ONLY. When attacking with a primary weapon from your primary firing arc, you may roll 1 additional attack die. If you do not, you may perform an additional attack from your auxiliary firing arc.</t>
+  </si>
+  <si>
+    <t>U0071</t>
+  </si>
+  <si>
+    <t>U0072</t>
+  </si>
+  <si>
+    <t>U0073</t>
+  </si>
+  <si>
+    <t>Bodyguard</t>
+  </si>
+  <si>
+    <t>SCUM ONLY. At the start of the combat phase, you may spend a focus token to choose a friendly ship at Range 1 with higher pilot skill than you. Increase its agility value by 1 until the end of the round.</t>
+  </si>
+  <si>
+    <t>Calculation</t>
+  </si>
+  <si>
+    <t>When attacking, you may spend 1 focus token to change 1 of your FOCUS results to a CRIT result.</t>
+  </si>
+  <si>
+    <t>Accuracy Corrector</t>
+  </si>
+  <si>
+    <t>When attacking, during the 'Modify Attack Dice' step, you may cancel all your dice results. If you do, you may add 2 HIT results to your roll. Your dice cannot be modified again during this attack.</t>
+  </si>
+  <si>
+    <t>Ion Torpedoes</t>
+  </si>
+  <si>
+    <t>FP: 4, RNG: 2-3 ATTACK (TARGET LOCK): Spend your target lock and discard this card to perform this attack. If this attack hits, the defender and each ship at range 1 of it receive 1 ion token.</t>
+  </si>
+  <si>
+    <t>Inertial Dampeners</t>
+  </si>
+  <si>
+    <t>When you reveal your maneuver, you may discard this card to instead perform a white [STAY 0] maneuver. Then receive 1 stress token.</t>
+  </si>
+  <si>
+    <t>Autothrusters</t>
+  </si>
+  <si>
+    <t>When defending, if you are beyond range 2 or outside the attacker's firing arc, you may change 1 of your blank results to an EVADE result. You can equip this card only if you have the BOOST action icon.</t>
+  </si>
+  <si>
+    <t>Hull Upgrade</t>
+  </si>
+  <si>
+    <t>Increase your hull value by 1.</t>
+  </si>
+  <si>
+    <t>Virago</t>
+  </si>
+  <si>
+    <t>STARVIPER ONLY. Your upgrade bar gains the SYSTEM and ILLICIT upgrade icons. You cannot equip this card if your pilot skill value is '3' or lower.</t>
+  </si>
+  <si>
+    <t>U0074</t>
+  </si>
+  <si>
+    <t>U0075</t>
+  </si>
+  <si>
+    <t>U0076</t>
+  </si>
+  <si>
+    <t>U0077</t>
+  </si>
+  <si>
+    <t>U0078</t>
+  </si>
+  <si>
+    <t>U0079</t>
+  </si>
+  <si>
+    <t>U0080</t>
+  </si>
+  <si>
+    <t>U0081</t>
+  </si>
+  <si>
+    <t>Homing Missiles</t>
+  </si>
+  <si>
+    <t>FP: 4, RNG: 2-3 ATTACK (TARGET LOCK): Discard this card to perform this attack. The defender cannot spend evade tokens during this attack.</t>
+  </si>
+  <si>
+    <t>Assault Missiles</t>
+  </si>
+  <si>
+    <t>FP: 4, RNG: 2-3 ATTACK (TARGET LOCK): Spend your target lock and discard this card to perform this attack. If this attack hits, each other ship at Range 1 of the defender suffers 1 damage.</t>
+  </si>
+  <si>
+    <t>Expose</t>
+  </si>
+  <si>
+    <t>ACTION: Until the end of the round, increase your primary weapon value 1, and decrease your agility value by 1.</t>
+  </si>
+  <si>
+    <t>Veteran Instincts</t>
+  </si>
+  <si>
+    <t>Increase your pilot skill value by 2.</t>
+  </si>
+  <si>
+    <t>Seismic Charges</t>
+  </si>
+  <si>
+    <t>When you reveal you maneuver dial, you may discard this card to DROP 1 seismic charge token. This token DETONATES at the end of the activation phase.</t>
+  </si>
+  <si>
+    <t>Stealth Device</t>
+  </si>
+  <si>
+    <t>Increase your agility value by 1. If you are hit by an attack, discard this card.</t>
+  </si>
+  <si>
+    <t>Mercenary Copilot</t>
+  </si>
+  <si>
+    <t>When attacking at Range 3, you may change 1 of your HIT results to a CRIT result.</t>
+  </si>
+  <si>
+    <t>Gunner</t>
+  </si>
+  <si>
+    <t>After you perform and attack that does not hit, you may immediately perform a primary weapon attack. You cannot perform another attack this round.</t>
+  </si>
+  <si>
+    <t>Slave 1</t>
+  </si>
+  <si>
+    <t>FIRESPRAY-31 ONLY. Your upgrade bar gains the TORPEDO upgrade icon.</t>
+  </si>
+  <si>
+    <t>U0082</t>
+  </si>
+  <si>
+    <t>U0083</t>
+  </si>
+  <si>
+    <t>U0084</t>
+  </si>
+  <si>
+    <t>U0085</t>
+  </si>
+  <si>
+    <t>U0086</t>
+  </si>
+  <si>
+    <t>U0087</t>
+  </si>
+  <si>
+    <t>U0088</t>
+  </si>
+  <si>
+    <t>U0089</t>
+  </si>
+  <si>
+    <t>U0090</t>
+  </si>
+  <si>
+    <t>Ruthlessness</t>
+  </si>
+  <si>
+    <t>IMPERIAL ONLY. After you perform an attack that hits, you MUST choose 1 other ship at Range 1 of the defender (other than yourself). That ship suffers 1 damage.</t>
+  </si>
+  <si>
+    <t>Intimidation</t>
+  </si>
+  <si>
+    <t>While you are touching an enemy ship, reduce that ship's agility value by 1.</t>
+  </si>
+  <si>
+    <t>Fleet Officer</t>
+  </si>
+  <si>
+    <t>IMPERIAL ONLY. ACTION: choose up to 2 friendly ships at Range 1-2 and assign 1 focus token to each of those ships. Then receive 1 stress token.</t>
+  </si>
+  <si>
+    <t>Mara Jade</t>
+  </si>
+  <si>
+    <t>IMPERIAL ONLY. At the end of the Combat phase, each enemy shipat Range 1 that does not have a stress token receives 1 stress token.</t>
+  </si>
+  <si>
+    <t>Ysanne Isard</t>
+  </si>
+  <si>
+    <t>IMPERIAL ONLY. At the start of the Combat phase, if you have no shields and at least 1 Damage card assigned to your ship, you may perform a free evade action.</t>
+  </si>
+  <si>
+    <t>Moff Jerjerrod</t>
+  </si>
+  <si>
+    <t>IMPERIAL ONLY. When you are dealt a faceup Damage card, you may discard this Upgrade card or another CREW Upgrade card to flip that Damage card facedown (without resolving its effect).</t>
+  </si>
+  <si>
+    <t>Proton Bombs</t>
+  </si>
+  <si>
+    <t>When you reveal your maneuver dial, you may discard this card to DROP 1 proton bomb token. This token DETONATES at the end of the Activation phase.</t>
+  </si>
+  <si>
+    <t>Tactical Jammer</t>
+  </si>
+  <si>
+    <t>LARGE SHIP ONLY. Your ship can obstruct enemy attacks.</t>
+  </si>
+  <si>
+    <t>Dauntless</t>
+  </si>
+  <si>
+    <t>VT-49 DECIMATOR ONLY. After you execute a maneuver that causes you to overlap another ship, you may perform 1 free action. Then receive 1 stress token.</t>
+  </si>
+  <si>
+    <t>U0091</t>
+  </si>
+  <si>
+    <t>U0092</t>
+  </si>
+  <si>
+    <t>U0093</t>
+  </si>
+  <si>
+    <t>U0094</t>
+  </si>
+  <si>
+    <t>U0095</t>
+  </si>
+  <si>
+    <t>U0096</t>
+  </si>
+  <si>
+    <t>U0097</t>
+  </si>
+  <si>
+    <t>U0098</t>
+  </si>
+  <si>
+    <t>U0099</t>
+  </si>
+  <si>
+    <t>Trick Shot</t>
+  </si>
+  <si>
+    <t>When attacking, if the attack is obstructed, you may roll an additional attack die.</t>
+  </si>
+  <si>
+    <t>Finn</t>
+  </si>
+  <si>
+    <t>REBEL ONLY. When attacking with a primary weapon or defending, if the enemy ship is inside your firing arc, you may add 1 blank result to your roll.</t>
+  </si>
+  <si>
+    <t>Rey</t>
+  </si>
+  <si>
+    <t>REBEL ONLY. At the start of the End phase, you may place one of your ship's focus tokens on this card. At the start of the Combat phase, you may assign 1 of those tokens to your ship.</t>
+  </si>
+  <si>
+    <t>Hotshot Co-Pilot</t>
+  </si>
+  <si>
+    <t>When attacking with a primary weapon, the defender must spend 1 focus token if able. When defending, the attacker must spend 1 focus token if able.</t>
+  </si>
+  <si>
+    <t>Snap Shot</t>
+  </si>
+  <si>
+    <t>FP: 2, RNG: 1  After an enemy ship executes a maneuver, you may perform this attack against that ship. ATTACK: Attack 1 ship. You cannot modify your attack dice and cannot attack again this phase.</t>
+  </si>
+  <si>
+    <t>M9-G8</t>
+  </si>
+  <si>
+    <t>When a ship you have locked is attacking, you may choose 1 attack die. The attacker must reroll that die. You can acquire target locks on other friendly ships.</t>
+  </si>
+  <si>
+    <t>Burnout SLAM</t>
+  </si>
+  <si>
+    <t>LARGE SHIP ONLY. Your action bar gains the SLAM action icon. After you perform a SLAM action, discard this card.</t>
+  </si>
+  <si>
+    <t>Primed Thrusters</t>
+  </si>
+  <si>
+    <t>SMALL SHIP ONLY. Stress tokens do not prevent you from performing boost or barrel roll actions unless you have 3 or more stress tokens.</t>
+  </si>
+  <si>
+    <t>Pattern Analyzer</t>
+  </si>
+  <si>
+    <t>When executing a maneuver, you may resolve the 'Check Pilot Stress' step after the 'Perform Action' step (instead of before that step).</t>
+  </si>
+  <si>
+    <t>Millenium Falcon</t>
+  </si>
+  <si>
+    <t>YT-1300 ONLY. After you execute a 3-speed bank maneuver, if you are not touching another ship and you are not stressed, you may receive 1 stress token to rotate your ship 180 degrees.</t>
+  </si>
+  <si>
+    <t>Black One</t>
+  </si>
+  <si>
+    <t>T-70 X-WING ONLY. After you perform a boost or barrel roll action, you may remove 1 enemy target lock from a friendly ship at range 1. You cannot equip this card if your pilot skill is '6' or lower.</t>
+  </si>
+  <si>
+    <t>Smuggling Compartment</t>
+  </si>
+  <si>
+    <t>YT-1300 OR YT-2400 ONLY. Your upgrade bar gains the ILLICIT icon. You may equip 1 additional Modification upgrade that costs 3 or fewer squad points.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -1219,19 +1552,19 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3F9499D8-5CE4-4AC7-B597-31CD0CBB4E0C}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="36.88671875" customWidth="1"/>
+    <col min="2" max="2" width="36.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>36</v>
       </c>
@@ -1242,7 +1575,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>50</v>
       </c>
@@ -1253,7 +1586,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>51</v>
       </c>
@@ -1264,7 +1597,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>52</v>
       </c>
@@ -1275,7 +1608,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>53</v>
       </c>
@@ -1286,7 +1619,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>54</v>
       </c>
@@ -1297,7 +1630,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>55</v>
       </c>
@@ -1308,7 +1641,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>56</v>
       </c>
@@ -1319,7 +1652,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>57</v>
       </c>
@@ -1330,7 +1663,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>58</v>
       </c>
@@ -1341,7 +1674,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>59</v>
       </c>
@@ -1359,20 +1692,20 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{258C231B-D951-459D-84CF-A781BDBA3B3B}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M4"/>
   <sheetViews>
     <sheetView topLeftCell="I1" workbookViewId="0">
       <selection activeCell="M5" sqref="M5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="3" width="26.6640625" customWidth="1"/>
-    <col min="4" max="4" width="14.5546875" customWidth="1"/>
+    <col min="2" max="3" width="26.7109375" customWidth="1"/>
+    <col min="4" max="4" width="14.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>36</v>
       </c>
@@ -1413,7 +1746,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>42</v>
       </c>
@@ -1454,7 +1787,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>43</v>
       </c>
@@ -1495,7 +1828,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>44</v>
       </c>
@@ -1543,23 +1876,23 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{18EF0634-2CFE-451C-B280-271F73D0B3E3}">
-  <dimension ref="A1:H71"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:H112"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A58" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A63" sqref="A63:A71"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A90" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B113" sqref="B113"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="7.44140625" customWidth="1"/>
-    <col min="2" max="2" width="21.109375" customWidth="1"/>
-    <col min="3" max="3" width="126.77734375" style="2" customWidth="1"/>
-    <col min="7" max="7" width="13.21875" customWidth="1"/>
+    <col min="1" max="1" width="7.42578125" customWidth="1"/>
+    <col min="2" max="2" width="21.140625" customWidth="1"/>
+    <col min="3" max="3" width="126.7109375" style="2" customWidth="1"/>
+    <col min="7" max="7" width="13.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>36</v>
       </c>
@@ -1585,7 +1918,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="s">
         <v>45</v>
       </c>
@@ -1611,7 +1944,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A3" s="5" t="s">
         <v>46</v>
       </c>
@@ -1637,7 +1970,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A4" s="5" t="s">
         <v>47</v>
       </c>
@@ -1663,7 +1996,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A5" s="5" t="s">
         <v>48</v>
       </c>
@@ -1689,7 +2022,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="6" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A6" s="5" t="s">
         <v>84</v>
       </c>
@@ -1715,7 +2048,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="7" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A7" s="5" t="s">
         <v>85</v>
       </c>
@@ -1741,7 +2074,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="8" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A8" s="5" t="s">
         <v>86</v>
       </c>
@@ -1767,7 +2100,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" s="5" t="s">
         <v>87</v>
       </c>
@@ -1793,7 +2126,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A10" s="5" t="s">
         <v>88</v>
       </c>
@@ -1819,7 +2152,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A11" s="5" t="s">
         <v>89</v>
       </c>
@@ -1845,7 +2178,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A12" s="5" t="s">
         <v>90</v>
       </c>
@@ -1871,7 +2204,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" s="5" t="s">
         <v>121</v>
       </c>
@@ -1897,7 +2230,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14" s="5" t="s">
         <v>122</v>
       </c>
@@ -1923,7 +2256,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15" s="5" t="s">
         <v>123</v>
       </c>
@@ -1949,7 +2282,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16" s="5" t="s">
         <v>124</v>
       </c>
@@ -1975,7 +2308,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A17" s="5" t="s">
         <v>125</v>
       </c>
@@ -2001,7 +2334,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A18" s="5" t="s">
         <v>126</v>
       </c>
@@ -2027,7 +2360,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A19" s="5" t="s">
         <v>127</v>
       </c>
@@ -2053,7 +2386,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A20" s="5" t="s">
         <v>128</v>
       </c>
@@ -2079,7 +2412,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="21" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A21" s="5" t="s">
         <v>129</v>
       </c>
@@ -2105,7 +2438,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A22" s="5" t="s">
         <v>130</v>
       </c>
@@ -2131,7 +2464,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="23" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A23" s="5" t="s">
         <v>131</v>
       </c>
@@ -2157,7 +2490,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="24" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A24" s="5" t="s">
         <v>132</v>
       </c>
@@ -2183,7 +2516,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="25" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A25" s="5" t="s">
         <v>133</v>
       </c>
@@ -2209,7 +2542,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A26" s="5" t="s">
         <v>134</v>
       </c>
@@ -2235,7 +2568,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A27" s="5" t="s">
         <v>157</v>
       </c>
@@ -2261,7 +2594,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A28" s="5" t="s">
         <v>158</v>
       </c>
@@ -2287,7 +2620,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A29" s="5" t="s">
         <v>159</v>
       </c>
@@ -2313,7 +2646,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A30" s="5" t="s">
         <v>160</v>
       </c>
@@ -2339,7 +2672,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="31" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A31" s="5" t="s">
         <v>161</v>
       </c>
@@ -2365,7 +2698,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="32" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A32" s="5" t="s">
         <v>162</v>
       </c>
@@ -2391,7 +2724,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="33" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A33" s="5" t="s">
         <v>163</v>
       </c>
@@ -2417,7 +2750,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="34" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A34" s="5" t="s">
         <v>164</v>
       </c>
@@ -2443,7 +2776,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="35" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A35" s="5" t="s">
         <v>165</v>
       </c>
@@ -2469,7 +2802,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="36" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A36" s="5" t="s">
         <v>166</v>
       </c>
@@ -2495,7 +2828,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="37" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A37" s="5" t="s">
         <v>167</v>
       </c>
@@ -2521,7 +2854,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="38" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A38" s="5" t="s">
         <v>188</v>
       </c>
@@ -2547,7 +2880,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="39" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A39" s="5" t="s">
         <v>189</v>
       </c>
@@ -2573,7 +2906,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="40" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A40" s="5" t="s">
         <v>190</v>
       </c>
@@ -2599,7 +2932,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="41" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A41" s="5" t="s">
         <v>191</v>
       </c>
@@ -2622,10 +2955,10 @@
         <v>22</v>
       </c>
       <c r="H41" s="5">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="42" spans="1:8" x14ac:dyDescent="0.3">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="42" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A42" s="5" t="s">
         <v>192</v>
       </c>
@@ -2651,7 +2984,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="43" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A43" s="5" t="s">
         <v>193</v>
       </c>
@@ -2677,7 +3010,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="44" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A44" s="5" t="s">
         <v>194</v>
       </c>
@@ -2703,7 +3036,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="45" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A45" s="5" t="s">
         <v>195</v>
       </c>
@@ -2729,7 +3062,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="46" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A46" s="5" t="s">
         <v>196</v>
       </c>
@@ -2755,7 +3088,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="47" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A47" s="5" t="s">
         <v>197</v>
       </c>
@@ -2781,7 +3114,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="48" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A48" s="5" t="s">
         <v>198</v>
       </c>
@@ -2807,7 +3140,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="49" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A49" s="5" t="s">
         <v>218</v>
       </c>
@@ -2830,10 +3163,10 @@
         <v>20</v>
       </c>
       <c r="H49" s="5">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="50" spans="1:8" x14ac:dyDescent="0.3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="50" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A50" s="5" t="s">
         <v>219</v>
       </c>
@@ -2859,7 +3192,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="51" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A51" s="5" t="s">
         <v>220</v>
       </c>
@@ -2885,7 +3218,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="52" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A52" s="5" t="s">
         <v>221</v>
       </c>
@@ -2911,7 +3244,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="53" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A53" s="5" t="s">
         <v>222</v>
       </c>
@@ -2937,7 +3270,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="54" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A54" s="5" t="s">
         <v>223</v>
       </c>
@@ -2963,7 +3296,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="55" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A55" s="5" t="s">
         <v>224</v>
       </c>
@@ -2989,7 +3322,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="56" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A56" s="5" t="s">
         <v>225</v>
       </c>
@@ -3015,7 +3348,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="57" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A57" s="5" t="s">
         <v>226</v>
       </c>
@@ -3041,7 +3374,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="58" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A58" s="5" t="s">
         <v>227</v>
       </c>
@@ -3067,7 +3400,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="59" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A59" s="5" t="s">
         <v>228</v>
       </c>
@@ -3093,7 +3426,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="60" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A60" s="5" t="s">
         <v>229</v>
       </c>
@@ -3116,10 +3449,10 @@
         <v>240</v>
       </c>
       <c r="H60" s="5">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="61" spans="1:8" x14ac:dyDescent="0.3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="61" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A61" s="5" t="s">
         <v>230</v>
       </c>
@@ -3142,10 +3475,10 @@
         <v>240</v>
       </c>
       <c r="H61" s="5">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="62" spans="1:8" x14ac:dyDescent="0.3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="62" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A62" s="5" t="s">
         <v>231</v>
       </c>
@@ -3171,7 +3504,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="63" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A63" s="5" t="s">
         <v>232</v>
       </c>
@@ -3197,7 +3530,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="64" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A64" s="5" t="s">
         <v>233</v>
       </c>
@@ -3223,7 +3556,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="65" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A65" s="5" t="s">
         <v>234</v>
       </c>
@@ -3246,10 +3579,10 @@
         <v>249</v>
       </c>
       <c r="H65" s="5">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="66" spans="1:8" x14ac:dyDescent="0.3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="66" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A66" s="5" t="s">
         <v>266</v>
       </c>
@@ -3275,7 +3608,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="67" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A67" s="5" t="s">
         <v>267</v>
       </c>
@@ -3301,7 +3634,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="68" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A68" s="5" t="s">
         <v>268</v>
       </c>
@@ -3327,7 +3660,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="69" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A69" s="5" t="s">
         <v>269</v>
       </c>
@@ -3353,7 +3686,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="70" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A70" s="5" t="s">
         <v>270</v>
       </c>
@@ -3379,7 +3712,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="71" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A71" s="5" t="s">
         <v>271</v>
       </c>
@@ -3403,6 +3736,1036 @@
       </c>
       <c r="H71" s="5">
         <v>2</v>
+      </c>
+    </row>
+    <row r="72" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="A72" s="5" t="s">
+        <v>278</v>
+      </c>
+      <c r="B72" s="5" t="s">
+        <v>272</v>
+      </c>
+      <c r="C72" s="2" t="s">
+        <v>273</v>
+      </c>
+      <c r="D72" s="5">
+        <v>0</v>
+      </c>
+      <c r="E72" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="F72" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="G72" s="5" t="s">
+        <v>83</v>
+      </c>
+      <c r="H72" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="73" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A73" s="5" t="s">
+        <v>279</v>
+      </c>
+      <c r="B73" s="5" t="s">
+        <v>274</v>
+      </c>
+      <c r="C73" s="2" t="s">
+        <v>275</v>
+      </c>
+      <c r="D73" s="5">
+        <v>2</v>
+      </c>
+      <c r="E73" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="F73" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="G73" s="5" t="s">
+        <v>99</v>
+      </c>
+      <c r="H73" s="5">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="74" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="A74" s="5" t="s">
+        <v>280</v>
+      </c>
+      <c r="B74" s="5" t="s">
+        <v>276</v>
+      </c>
+      <c r="C74" s="2" t="s">
+        <v>277</v>
+      </c>
+      <c r="D74" s="5">
+        <v>0</v>
+      </c>
+      <c r="E74" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="F74" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="G74" s="5" t="s">
+        <v>61</v>
+      </c>
+      <c r="H74" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="75" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="A75" s="5" t="s">
+        <v>297</v>
+      </c>
+      <c r="B75" s="5" t="s">
+        <v>281</v>
+      </c>
+      <c r="C75" s="2" t="s">
+        <v>282</v>
+      </c>
+      <c r="D75" s="5">
+        <v>2</v>
+      </c>
+      <c r="E75" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="F75" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="G75" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="H75" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="76" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A76" s="5" t="s">
+        <v>298</v>
+      </c>
+      <c r="B76" s="5" t="s">
+        <v>283</v>
+      </c>
+      <c r="C76" s="2" t="s">
+        <v>284</v>
+      </c>
+      <c r="D76" s="5">
+        <v>1</v>
+      </c>
+      <c r="E76" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="F76" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="G76" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="H76" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="77" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="A77" s="5" t="s">
+        <v>299</v>
+      </c>
+      <c r="B77" s="5" t="s">
+        <v>285</v>
+      </c>
+      <c r="C77" s="2" t="s">
+        <v>286</v>
+      </c>
+      <c r="D77" s="5">
+        <v>3</v>
+      </c>
+      <c r="E77" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="F77" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="G77" s="5" t="s">
+        <v>83</v>
+      </c>
+      <c r="H77" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="78" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="A78" s="5" t="s">
+        <v>300</v>
+      </c>
+      <c r="B78" s="5" t="s">
+        <v>287</v>
+      </c>
+      <c r="C78" s="2" t="s">
+        <v>288</v>
+      </c>
+      <c r="D78" s="5">
+        <v>5</v>
+      </c>
+      <c r="E78" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="F78" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="G78" s="5" t="s">
+        <v>259</v>
+      </c>
+      <c r="H78" s="5">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="79" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A79" s="5" t="s">
+        <v>301</v>
+      </c>
+      <c r="B79" s="5" t="s">
+        <v>289</v>
+      </c>
+      <c r="C79" s="2" t="s">
+        <v>290</v>
+      </c>
+      <c r="D79" s="5">
+        <v>1</v>
+      </c>
+      <c r="E79" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="F79" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="G79" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="H79" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="80" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="A80" s="5" t="s">
+        <v>302</v>
+      </c>
+      <c r="B80" s="5" t="s">
+        <v>291</v>
+      </c>
+      <c r="C80" s="2" t="s">
+        <v>292</v>
+      </c>
+      <c r="D80" s="5">
+        <v>2</v>
+      </c>
+      <c r="E80" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="F80" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="G80" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="H80" s="5">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="81" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A81" s="5" t="s">
+        <v>303</v>
+      </c>
+      <c r="B81" s="5" t="s">
+        <v>293</v>
+      </c>
+      <c r="C81" s="2" t="s">
+        <v>294</v>
+      </c>
+      <c r="D81" s="5">
+        <v>3</v>
+      </c>
+      <c r="E81" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="F81" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="G81" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="H81" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="82" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="A82" s="5" t="s">
+        <v>304</v>
+      </c>
+      <c r="B82" s="5" t="s">
+        <v>295</v>
+      </c>
+      <c r="C82" s="2" t="s">
+        <v>296</v>
+      </c>
+      <c r="D82" s="5">
+        <v>1</v>
+      </c>
+      <c r="E82" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="F82" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="G82" s="5" t="s">
+        <v>61</v>
+      </c>
+      <c r="H82" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="83" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="A83" s="5" t="s">
+        <v>323</v>
+      </c>
+      <c r="B83" s="5" t="s">
+        <v>305</v>
+      </c>
+      <c r="C83" s="2" t="s">
+        <v>306</v>
+      </c>
+      <c r="D83" s="5">
+        <v>5</v>
+      </c>
+      <c r="E83" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="F83" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="G83" s="5" t="s">
+        <v>254</v>
+      </c>
+      <c r="H83" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="84" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="A84" s="5" t="s">
+        <v>324</v>
+      </c>
+      <c r="B84" s="5" t="s">
+        <v>307</v>
+      </c>
+      <c r="C84" s="2" t="s">
+        <v>308</v>
+      </c>
+      <c r="D84" s="5">
+        <v>5</v>
+      </c>
+      <c r="E84" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="F84" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="G84" s="5" t="s">
+        <v>254</v>
+      </c>
+      <c r="H84" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="85" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A85" s="5" t="s">
+        <v>325</v>
+      </c>
+      <c r="B85" s="5" t="s">
+        <v>309</v>
+      </c>
+      <c r="C85" s="2" t="s">
+        <v>310</v>
+      </c>
+      <c r="D85" s="5">
+        <v>4</v>
+      </c>
+      <c r="E85" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="F85" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="G85" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="H85" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="86" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A86" s="5" t="s">
+        <v>326</v>
+      </c>
+      <c r="B86" s="5" t="s">
+        <v>311</v>
+      </c>
+      <c r="C86" s="2" t="s">
+        <v>312</v>
+      </c>
+      <c r="D86" s="5">
+        <v>1</v>
+      </c>
+      <c r="E86" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="F86" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="G86" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="H86" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="87" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="A87" s="5" t="s">
+        <v>327</v>
+      </c>
+      <c r="B87" s="5" t="s">
+        <v>313</v>
+      </c>
+      <c r="C87" s="2" t="s">
+        <v>314</v>
+      </c>
+      <c r="D87" s="5">
+        <v>2</v>
+      </c>
+      <c r="E87" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="F87" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="G87" s="5" t="s">
+        <v>249</v>
+      </c>
+      <c r="H87" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="88" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A88" s="5" t="s">
+        <v>328</v>
+      </c>
+      <c r="B88" s="5" t="s">
+        <v>315</v>
+      </c>
+      <c r="C88" s="2" t="s">
+        <v>316</v>
+      </c>
+      <c r="D88" s="5">
+        <v>3</v>
+      </c>
+      <c r="E88" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="F88" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="G88" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="H88" s="5">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="89" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A89" s="5" t="s">
+        <v>329</v>
+      </c>
+      <c r="B89" s="5" t="s">
+        <v>317</v>
+      </c>
+      <c r="C89" s="2" t="s">
+        <v>318</v>
+      </c>
+      <c r="D89" s="5">
+        <v>2</v>
+      </c>
+      <c r="E89" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="F89" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="G89" s="5" t="s">
+        <v>137</v>
+      </c>
+      <c r="H89" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="90" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="A90" s="5" t="s">
+        <v>330</v>
+      </c>
+      <c r="B90" s="5" t="s">
+        <v>319</v>
+      </c>
+      <c r="C90" s="2" t="s">
+        <v>320</v>
+      </c>
+      <c r="D90" s="5">
+        <v>5</v>
+      </c>
+      <c r="E90" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="F90" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="G90" s="5" t="s">
+        <v>137</v>
+      </c>
+      <c r="H90" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="91" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A91" s="5" t="s">
+        <v>331</v>
+      </c>
+      <c r="B91" s="5" t="s">
+        <v>321</v>
+      </c>
+      <c r="C91" s="2" t="s">
+        <v>322</v>
+      </c>
+      <c r="D91" s="5">
+        <v>0</v>
+      </c>
+      <c r="E91" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="F91" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="G91" s="5" t="s">
+        <v>61</v>
+      </c>
+      <c r="H91" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="92" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="A92" s="5" t="s">
+        <v>350</v>
+      </c>
+      <c r="B92" s="5" t="s">
+        <v>332</v>
+      </c>
+      <c r="C92" s="2" t="s">
+        <v>333</v>
+      </c>
+      <c r="D92" s="5">
+        <v>3</v>
+      </c>
+      <c r="E92" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="F92" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="G92" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="H92" s="5">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="93" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A93" s="5" t="s">
+        <v>351</v>
+      </c>
+      <c r="B93" s="5" t="s">
+        <v>334</v>
+      </c>
+      <c r="C93" s="2" t="s">
+        <v>335</v>
+      </c>
+      <c r="D93" s="5">
+        <v>2</v>
+      </c>
+      <c r="E93" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="F93" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="G93" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="H93" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="94" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="A94" s="5" t="s">
+        <v>352</v>
+      </c>
+      <c r="B94" s="5" t="s">
+        <v>336</v>
+      </c>
+      <c r="C94" s="2" t="s">
+        <v>337</v>
+      </c>
+      <c r="D94" s="5">
+        <v>3</v>
+      </c>
+      <c r="E94" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="F94" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="G94" s="5" t="s">
+        <v>137</v>
+      </c>
+      <c r="H94" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="95" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A95" s="5" t="s">
+        <v>353</v>
+      </c>
+      <c r="B95" s="5" t="s">
+        <v>338</v>
+      </c>
+      <c r="C95" s="2" t="s">
+        <v>339</v>
+      </c>
+      <c r="D95" s="5">
+        <v>3</v>
+      </c>
+      <c r="E95" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="F95" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="G95" s="5" t="s">
+        <v>137</v>
+      </c>
+      <c r="H95" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="96" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="A96" s="5" t="s">
+        <v>354</v>
+      </c>
+      <c r="B96" s="5" t="s">
+        <v>340</v>
+      </c>
+      <c r="C96" s="2" t="s">
+        <v>341</v>
+      </c>
+      <c r="D96" s="5">
+        <v>4</v>
+      </c>
+      <c r="E96" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="F96" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="G96" s="5" t="s">
+        <v>137</v>
+      </c>
+      <c r="H96" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="97" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="A97" s="5" t="s">
+        <v>355</v>
+      </c>
+      <c r="B97" s="5" t="s">
+        <v>342</v>
+      </c>
+      <c r="C97" s="2" t="s">
+        <v>343</v>
+      </c>
+      <c r="D97" s="5">
+        <v>2</v>
+      </c>
+      <c r="E97" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="F97" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="G97" s="5" t="s">
+        <v>137</v>
+      </c>
+      <c r="H97" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="98" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="A98" s="5" t="s">
+        <v>356</v>
+      </c>
+      <c r="B98" s="5" t="s">
+        <v>344</v>
+      </c>
+      <c r="C98" s="2" t="s">
+        <v>345</v>
+      </c>
+      <c r="D98" s="5">
+        <v>5</v>
+      </c>
+      <c r="E98" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="F98" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="G98" s="5" t="s">
+        <v>249</v>
+      </c>
+      <c r="H98" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="99" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A99" s="5" t="s">
+        <v>357</v>
+      </c>
+      <c r="B99" s="5" t="s">
+        <v>346</v>
+      </c>
+      <c r="C99" s="2" t="s">
+        <v>347</v>
+      </c>
+      <c r="D99" s="5">
+        <v>1</v>
+      </c>
+      <c r="E99" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="F99" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="G99" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="H99" s="5">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="100" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="A100" s="5" t="s">
+        <v>358</v>
+      </c>
+      <c r="B100" s="5" t="s">
+        <v>348</v>
+      </c>
+      <c r="C100" s="2" t="s">
+        <v>349</v>
+      </c>
+      <c r="D100" s="5">
+        <v>2</v>
+      </c>
+      <c r="E100" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="F100" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="G100" s="5" t="s">
+        <v>61</v>
+      </c>
+      <c r="H100" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="101" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B101" s="5" t="s">
+        <v>359</v>
+      </c>
+      <c r="C101" s="2" t="s">
+        <v>360</v>
+      </c>
+      <c r="D101" s="5">
+        <v>0</v>
+      </c>
+      <c r="E101" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="F101" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="G101" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="H101" s="5">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="102" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="B102" s="5" t="s">
+        <v>361</v>
+      </c>
+      <c r="C102" s="2" t="s">
+        <v>362</v>
+      </c>
+      <c r="D102" s="5">
+        <v>5</v>
+      </c>
+      <c r="E102" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="F102" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="G102" s="5" t="s">
+        <v>137</v>
+      </c>
+      <c r="H102" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="103" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="B103" s="5" t="s">
+        <v>363</v>
+      </c>
+      <c r="C103" s="2" t="s">
+        <v>364</v>
+      </c>
+      <c r="D103" s="5">
+        <v>2</v>
+      </c>
+      <c r="E103" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="F103" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="G103" s="5" t="s">
+        <v>137</v>
+      </c>
+      <c r="H103" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="104" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="B104" s="5" t="s">
+        <v>365</v>
+      </c>
+      <c r="C104" s="2" t="s">
+        <v>366</v>
+      </c>
+      <c r="D104" s="5">
+        <v>4</v>
+      </c>
+      <c r="E104" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="F104" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="G104" s="5" t="s">
+        <v>137</v>
+      </c>
+      <c r="H104" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="105" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="B105" s="5" t="s">
+        <v>367</v>
+      </c>
+      <c r="C105" s="2" t="s">
+        <v>368</v>
+      </c>
+      <c r="D105" s="5">
+        <v>2</v>
+      </c>
+      <c r="E105" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="F105" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="G105" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="H105" s="5">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="106" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="B106" s="5" t="s">
+        <v>369</v>
+      </c>
+      <c r="C106" s="2" t="s">
+        <v>370</v>
+      </c>
+      <c r="D106" s="5">
+        <v>3</v>
+      </c>
+      <c r="E106" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="F106" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="G106" s="5" t="s">
+        <v>104</v>
+      </c>
+      <c r="H106" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="107" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B107" s="5" t="s">
+        <v>371</v>
+      </c>
+      <c r="C107" s="2" t="s">
+        <v>372</v>
+      </c>
+      <c r="D107" s="5">
+        <v>1</v>
+      </c>
+      <c r="E107" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="F107" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="G107" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="H107" s="5">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="108" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B108" s="5" t="s">
+        <v>373</v>
+      </c>
+      <c r="C108" s="2" t="s">
+        <v>374</v>
+      </c>
+      <c r="D108" s="5">
+        <v>1</v>
+      </c>
+      <c r="E108" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="F108" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="G108" s="5" t="s">
+        <v>99</v>
+      </c>
+      <c r="H108" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="109" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B109" s="5" t="s">
+        <v>375</v>
+      </c>
+      <c r="C109" s="2" t="s">
+        <v>376</v>
+      </c>
+      <c r="D109" s="5">
+        <v>2</v>
+      </c>
+      <c r="E109" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="F109" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="G109" s="5" t="s">
+        <v>99</v>
+      </c>
+      <c r="H109" s="5">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="110" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="B110" s="5" t="s">
+        <v>377</v>
+      </c>
+      <c r="C110" s="2" t="s">
+        <v>378</v>
+      </c>
+      <c r="D110" s="5">
+        <v>1</v>
+      </c>
+      <c r="E110" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="F110" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="G110" s="5" t="s">
+        <v>61</v>
+      </c>
+      <c r="H110" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="111" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="B111" s="5" t="s">
+        <v>379</v>
+      </c>
+      <c r="C111" s="2" t="s">
+        <v>380</v>
+      </c>
+      <c r="D111" s="5">
+        <v>1</v>
+      </c>
+      <c r="E111" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="F111" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="G111" s="5" t="s">
+        <v>61</v>
+      </c>
+      <c r="H111" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="112" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="B112" s="5" t="s">
+        <v>381</v>
+      </c>
+      <c r="C112" s="2" t="s">
+        <v>382</v>
+      </c>
+      <c r="D112" s="5">
+        <v>0</v>
+      </c>
+      <c r="E112" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="F112" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="G112" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="H112" s="5">
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>